<commit_message>
Update to new fuse and add alternative buzzer
</commit_message>
<xml_diff>
--- a/AxxSolder_hardware/bom/BOM_AxxSolder_V3_0.xlsx
+++ b/AxxSolder_hardware/bom/BOM_AxxSolder_V3_0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\axelj\ownCloud\2_Project\00_AxxProjects\AxxSolder\AxxSolder_hardware\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C738C754-9336-428A-9533-278C0B99A2E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{658BDA88-637D-4F2F-9C85-0A650135CE04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{60354D9D-8798-4211-B1E3-D5485177CC9B}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="245">
   <si>
     <t>References</t>
   </si>
@@ -756,6 +756,12 @@
   </si>
   <si>
     <t>https://eu.mouser.com/ProductDetail/Wurth-Elektronik/471001264143?qs=YCa%2FAAYMW03bZZ%252BoQThfXw%3D%3D</t>
+  </si>
+  <si>
+    <t>576-0154007.DR</t>
+  </si>
+  <si>
+    <t>0154007.DR</t>
   </si>
 </sst>
 </file>
@@ -5864,7 +5870,7 @@
   <dimension ref="A1:M79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M65" sqref="M65"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5965,7 +5971,8 @@
         <v>4.2999999999999997E-2</v>
       </c>
       <c r="I4" s="15">
-        <v>0.73</v>
+        <f>G4*H4</f>
+        <v>0.73099999999999998</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -5993,8 +6000,9 @@
       <c r="H5" s="16">
         <v>0.17699999999999999</v>
       </c>
-      <c r="I5" s="16">
-        <v>2.83</v>
+      <c r="I5" s="15">
+        <f t="shared" ref="I5:I45" si="0">G5*H5</f>
+        <v>2.8319999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6023,7 +6031,8 @@
         <v>9.2999999999999999E-2</v>
       </c>
       <c r="I6" s="15">
-        <v>0.19</v>
+        <f t="shared" si="0"/>
+        <v>0.186</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6051,8 +6060,9 @@
       <c r="H7" s="16">
         <v>0.61399999999999999</v>
       </c>
-      <c r="I7" s="16">
-        <v>0.61</v>
+      <c r="I7" s="15">
+        <f t="shared" si="0"/>
+        <v>0.61399999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -6081,6 +6091,7 @@
         <v>0.125</v>
       </c>
       <c r="I8" s="15">
+        <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
     </row>
@@ -6109,8 +6120,9 @@
       <c r="H9" s="16">
         <v>0.14000000000000001</v>
       </c>
-      <c r="I9" s="16">
-        <v>0.7</v>
+      <c r="I9" s="15">
+        <f t="shared" si="0"/>
+        <v>0.70000000000000007</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6139,7 +6151,8 @@
         <v>0.214</v>
       </c>
       <c r="I10" s="15">
-        <v>0.86</v>
+        <f t="shared" si="0"/>
+        <v>0.85599999999999998</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6167,8 +6180,9 @@
       <c r="H11" s="16">
         <v>0.121</v>
       </c>
-      <c r="I11" s="16">
-        <v>0.48</v>
+      <c r="I11" s="15">
+        <f t="shared" si="0"/>
+        <v>0.48399999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6197,7 +6211,8 @@
         <v>0.121</v>
       </c>
       <c r="I12" s="15">
-        <v>0.24</v>
+        <f t="shared" si="0"/>
+        <v>0.24199999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6225,8 +6240,9 @@
       <c r="H13" s="16">
         <v>0.307</v>
       </c>
-      <c r="I13" s="16">
-        <v>0.61</v>
+      <c r="I13" s="15">
+        <f t="shared" si="0"/>
+        <v>0.61399999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6255,7 +6271,8 @@
         <v>0.753</v>
       </c>
       <c r="I14" s="15">
-        <v>0.75</v>
+        <f t="shared" si="0"/>
+        <v>0.753</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6283,8 +6300,9 @@
       <c r="H15" s="16">
         <v>9.2999999999999999E-2</v>
       </c>
-      <c r="I15" s="16">
-        <v>0.09</v>
+      <c r="I15" s="15">
+        <f t="shared" si="0"/>
+        <v>9.2999999999999999E-2</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6313,7 +6331,8 @@
         <v>0.36299999999999999</v>
       </c>
       <c r="I16" s="15">
-        <v>0.36</v>
+        <f t="shared" si="0"/>
+        <v>0.36299999999999999</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6341,8 +6360,9 @@
       <c r="H17" s="16">
         <v>0.753</v>
       </c>
-      <c r="I17" s="16">
-        <v>0.75</v>
+      <c r="I17" s="15">
+        <f t="shared" si="0"/>
+        <v>0.753</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6371,7 +6391,8 @@
         <v>0.112</v>
       </c>
       <c r="I18" s="15">
-        <v>0.45</v>
+        <f t="shared" si="0"/>
+        <v>0.44800000000000001</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6399,7 +6420,8 @@
       <c r="H19" s="16">
         <v>0.19500000000000001</v>
       </c>
-      <c r="I19" s="16">
+      <c r="I19" s="15">
+        <f t="shared" si="0"/>
         <v>0.39</v>
       </c>
       <c r="K19" s="14"/>
@@ -6431,6 +6453,7 @@
         <v>0.4</v>
       </c>
       <c r="I20" s="15">
+        <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
       <c r="K20" s="14"/>
@@ -6461,8 +6484,9 @@
       <c r="H21" s="16">
         <v>0.372</v>
       </c>
-      <c r="I21" s="16">
-        <v>0.74</v>
+      <c r="I21" s="15">
+        <f t="shared" si="0"/>
+        <v>0.74399999999999999</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6491,6 +6515,7 @@
         <v>18.55</v>
       </c>
       <c r="I22" s="15">
+        <f t="shared" si="0"/>
         <v>18.55</v>
       </c>
     </row>
@@ -6519,7 +6544,8 @@
       <c r="H23" s="16">
         <v>2.37</v>
       </c>
-      <c r="I23" s="16">
+      <c r="I23" s="15">
+        <f t="shared" si="0"/>
         <v>2.37</v>
       </c>
     </row>
@@ -6549,6 +6575,7 @@
         <v>1.6</v>
       </c>
       <c r="I24" s="15">
+        <f t="shared" si="0"/>
         <v>1.6</v>
       </c>
     </row>
@@ -6557,7 +6584,7 @@
         <v>74</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>75</v>
+        <v>244</v>
       </c>
       <c r="C25" s="12" t="s">
         <v>76</v>
@@ -6566,19 +6593,20 @@
         <v>57</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>75</v>
+        <v>244</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>77</v>
+        <v>243</v>
       </c>
       <c r="G25" s="12">
         <v>1</v>
       </c>
       <c r="H25" s="16">
-        <v>2.99</v>
-      </c>
-      <c r="I25" s="16">
-        <v>2.99</v>
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="I25" s="15">
+        <f t="shared" si="0"/>
+        <v>2.5499999999999998</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6607,7 +6635,8 @@
         <v>0.72499999999999998</v>
       </c>
       <c r="I26" s="15">
-        <v>0.73</v>
+        <f t="shared" si="0"/>
+        <v>0.72499999999999998</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6635,8 +6664,9 @@
       <c r="H27" s="16">
         <v>0.54900000000000004</v>
       </c>
-      <c r="I27" s="16">
-        <v>1.65</v>
+      <c r="I27" s="15">
+        <f t="shared" si="0"/>
+        <v>1.6470000000000002</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6665,7 +6695,8 @@
         <v>0.17699999999999999</v>
       </c>
       <c r="I28" s="15">
-        <v>0.18</v>
+        <f t="shared" si="0"/>
+        <v>0.17699999999999999</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6693,8 +6724,9 @@
       <c r="H29" s="16">
         <v>0.38100000000000001</v>
       </c>
-      <c r="I29" s="16">
-        <v>0.38</v>
+      <c r="I29" s="15">
+        <f t="shared" si="0"/>
+        <v>0.38100000000000001</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6723,6 +6755,7 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="I30" s="15">
+        <f t="shared" si="0"/>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -6751,8 +6784,9 @@
       <c r="H31" s="16">
         <v>0.96699999999999997</v>
       </c>
-      <c r="I31" s="16">
-        <v>0.97</v>
+      <c r="I31" s="15">
+        <f t="shared" si="0"/>
+        <v>0.96699999999999997</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6781,6 +6815,7 @@
         <v>5.65</v>
       </c>
       <c r="I32" s="15">
+        <f t="shared" si="0"/>
         <v>5.65</v>
       </c>
     </row>
@@ -6809,8 +6844,9 @@
       <c r="H33" s="16">
         <v>0.32600000000000001</v>
       </c>
-      <c r="I33" s="16">
-        <v>0.33</v>
+      <c r="I33" s="15">
+        <f t="shared" si="0"/>
+        <v>0.32600000000000001</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6839,6 +6875,7 @@
         <v>2.52</v>
       </c>
       <c r="I34" s="15">
+        <f t="shared" si="0"/>
         <v>2.52</v>
       </c>
     </row>
@@ -6867,7 +6904,8 @@
       <c r="H35" s="16">
         <v>2.64</v>
       </c>
-      <c r="I35" s="16">
+      <c r="I35" s="15">
+        <f t="shared" si="0"/>
         <v>2.64</v>
       </c>
     </row>
@@ -6897,6 +6935,7 @@
         <v>5.22</v>
       </c>
       <c r="I36" s="15">
+        <f t="shared" si="0"/>
         <v>5.22</v>
       </c>
     </row>
@@ -6925,8 +6964,9 @@
       <c r="H37" s="16">
         <v>0.81799999999999995</v>
       </c>
-      <c r="I37" s="16">
-        <v>0.82</v>
+      <c r="I37" s="15">
+        <f t="shared" si="0"/>
+        <v>0.81799999999999995</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6955,6 +6995,7 @@
         <v>2.71</v>
       </c>
       <c r="I38" s="15">
+        <f t="shared" si="0"/>
         <v>2.71</v>
       </c>
     </row>
@@ -6983,8 +7024,9 @@
       <c r="H39" s="16">
         <v>0.995</v>
       </c>
-      <c r="I39" s="16">
-        <v>1</v>
+      <c r="I39" s="15">
+        <f t="shared" si="0"/>
+        <v>0.995</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7013,7 +7055,8 @@
         <v>0.96699999999999997</v>
       </c>
       <c r="I40" s="15">
-        <v>0.97</v>
+        <f t="shared" si="0"/>
+        <v>0.96699999999999997</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7041,7 +7084,8 @@
       <c r="H41" s="16">
         <v>0.13</v>
       </c>
-      <c r="I41" s="16">
+      <c r="I41" s="15">
+        <f t="shared" si="0"/>
         <v>0.13</v>
       </c>
     </row>
@@ -7071,7 +7115,8 @@
         <v>9.2999999999999999E-2</v>
       </c>
       <c r="I42" s="15">
-        <v>0.19</v>
+        <f t="shared" si="0"/>
+        <v>0.186</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7099,7 +7144,8 @@
       <c r="H43" s="16">
         <v>1.26</v>
       </c>
-      <c r="I43" s="16">
+      <c r="I43" s="15">
+        <f t="shared" si="0"/>
         <v>1.26</v>
       </c>
     </row>
@@ -7129,6 +7175,7 @@
         <v>3.7</v>
       </c>
       <c r="I44" s="15">
+        <f t="shared" si="0"/>
         <v>3.7</v>
       </c>
     </row>
@@ -7157,8 +7204,9 @@
       <c r="H45" s="16">
         <v>0.33500000000000002</v>
       </c>
-      <c r="I45" s="16">
-        <v>0.34</v>
+      <c r="I45" s="15">
+        <f t="shared" si="0"/>
+        <v>0.33500000000000002</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
@@ -7172,7 +7220,7 @@
       <c r="F46" s="7"/>
       <c r="I46" s="8">
         <f>SUM(I4:I45)</f>
-        <v>75.38</v>
+        <v>74.927000000000007</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
@@ -7254,7 +7302,7 @@
         <v>0.94899999999999995</v>
       </c>
       <c r="G52" s="9">
-        <f t="shared" ref="G52:G64" si="0">F52*E52</f>
+        <f t="shared" ref="G52:G64" si="1">F52*E52</f>
         <v>1.8979999999999999</v>
       </c>
     </row>
@@ -7272,7 +7320,7 @@
         <v>1.37</v>
       </c>
       <c r="G53" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.74</v>
       </c>
     </row>
@@ -7290,7 +7338,7 @@
         <v>0.84</v>
       </c>
       <c r="G54" s="9">
-        <f t="shared" ref="G54" si="1">F54*E54</f>
+        <f t="shared" ref="G54" si="2">F54*E54</f>
         <v>1.68</v>
       </c>
     </row>
@@ -7308,7 +7356,7 @@
         <v>0.875</v>
       </c>
       <c r="G55" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.875</v>
       </c>
     </row>
@@ -7326,7 +7374,7 @@
         <v>0.85599999999999998</v>
       </c>
       <c r="G56" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.712</v>
       </c>
     </row>
@@ -7344,7 +7392,7 @@
         <v>3.45</v>
       </c>
       <c r="G57" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.45</v>
       </c>
     </row>
@@ -7359,7 +7407,7 @@
         <v>5</v>
       </c>
       <c r="G58" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
     </row>
@@ -7377,7 +7425,7 @@
         <v>0.1</v>
       </c>
       <c r="G59" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
     </row>
@@ -7395,7 +7443,7 @@
         <v>0.1</v>
       </c>
       <c r="G60" s="9">
-        <f t="shared" ref="G60" si="2">F60*E60</f>
+        <f t="shared" ref="G60" si="3">F60*E60</f>
         <v>0.1</v>
       </c>
     </row>
@@ -7431,7 +7479,7 @@
         <v>0.1</v>
       </c>
       <c r="G62" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
     </row>
@@ -7449,7 +7497,7 @@
         <v>0.1</v>
       </c>
       <c r="G63" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
     </row>
@@ -7467,7 +7515,7 @@
         <v>1</v>
       </c>
       <c r="G64" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -7556,7 +7604,7 @@
         <v>66.34</v>
       </c>
       <c r="G74">
-        <f t="shared" ref="G74:G75" si="3">F74*E74</f>
+        <f t="shared" ref="G74:G75" si="4">F74*E74</f>
         <v>66.34</v>
       </c>
     </row>
@@ -7571,7 +7619,7 @@
         <v>38.340000000000003</v>
       </c>
       <c r="G75">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>38.340000000000003</v>
       </c>
     </row>
@@ -7595,7 +7643,7 @@
       <c r="E78" s="11"/>
       <c r="F78" s="20">
         <f>F76+G65+I46+G68</f>
-        <v>395.15499999999997</v>
+        <v>394.702</v>
       </c>
       <c r="G78" s="20"/>
     </row>
@@ -7609,7 +7657,7 @@
       <c r="E79" s="11"/>
       <c r="F79" s="20">
         <f>F76+G65+I46+G71</f>
-        <v>258.815</v>
+        <v>258.36200000000002</v>
       </c>
       <c r="G79" s="20"/>
     </row>
@@ -8751,7 +8799,2057 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2049" r:id="rId3" name="Control 1">
+        <control shapeId="2132" r:id="rId3" name="Control 84">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>41</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>41</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2132" r:id="rId3" name="Control 84"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2131" r:id="rId5" name="Control 83">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>41</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>41</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2131" r:id="rId5" name="Control 83"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2130" r:id="rId6" name="Control 82">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>40</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>40</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2130" r:id="rId6" name="Control 82"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2129" r:id="rId7" name="Control 81">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>40</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>40</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2129" r:id="rId7" name="Control 81"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2128" r:id="rId8" name="Control 80">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>39</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>39</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2128" r:id="rId8" name="Control 80"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2127" r:id="rId9" name="Control 79">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>39</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>39</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2127" r:id="rId9" name="Control 79"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2126" r:id="rId10" name="Control 78">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>38</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>38</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2126" r:id="rId10" name="Control 78"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2125" r:id="rId11" name="Control 77">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>38</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>38</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2125" r:id="rId11" name="Control 77"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2124" r:id="rId12" name="Control 76">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>37</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>37</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2124" r:id="rId12" name="Control 76"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2123" r:id="rId13" name="Control 75">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>37</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>37</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2123" r:id="rId13" name="Control 75"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2122" r:id="rId14" name="Control 74">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>36</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>36</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2122" r:id="rId14" name="Control 74"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2121" r:id="rId15" name="Control 73">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>36</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>36</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2121" r:id="rId15" name="Control 73"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2120" r:id="rId16" name="Control 72">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>35</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>35</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2120" r:id="rId16" name="Control 72"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2119" r:id="rId17" name="Control 71">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>35</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>35</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2119" r:id="rId17" name="Control 71"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2118" r:id="rId18" name="Control 70">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>34</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>34</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2118" r:id="rId18" name="Control 70"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2117" r:id="rId19" name="Control 69">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>34</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>34</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2117" r:id="rId19" name="Control 69"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2116" r:id="rId20" name="Control 68">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>33</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>33</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2116" r:id="rId20" name="Control 68"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2115" r:id="rId21" name="Control 67">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>33</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>33</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2115" r:id="rId21" name="Control 67"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2114" r:id="rId22" name="Control 66">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>32</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>32</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2114" r:id="rId22" name="Control 66"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2113" r:id="rId23" name="Control 65">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>32</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>32</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2113" r:id="rId23" name="Control 65"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2112" r:id="rId24" name="Control 64">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>31</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>31</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2112" r:id="rId24" name="Control 64"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2111" r:id="rId25" name="Control 63">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>31</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>31</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2111" r:id="rId25" name="Control 63"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2110" r:id="rId26" name="Control 62">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>30</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>30</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2110" r:id="rId26" name="Control 62"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2109" r:id="rId27" name="Control 61">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>30</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>30</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2109" r:id="rId27" name="Control 61"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2108" r:id="rId28" name="Control 60">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>29</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>29</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2108" r:id="rId28" name="Control 60"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2107" r:id="rId29" name="Control 59">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>29</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>29</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2107" r:id="rId29" name="Control 59"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2106" r:id="rId30" name="Control 58">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>28</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>28</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2106" r:id="rId30" name="Control 58"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2105" r:id="rId31" name="Control 57">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>28</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>28</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2105" r:id="rId31" name="Control 57"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2104" r:id="rId32" name="Control 56">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>27</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>27</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2104" r:id="rId32" name="Control 56"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2103" r:id="rId33" name="Control 55">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>27</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>27</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2103" r:id="rId33" name="Control 55"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2102" r:id="rId34" name="Control 54">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>26</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>26</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2102" r:id="rId34" name="Control 54"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2101" r:id="rId35" name="Control 53">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>26</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>26</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2101" r:id="rId35" name="Control 53"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2100" r:id="rId36" name="Control 52">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>25</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>25</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2100" r:id="rId36" name="Control 52"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2099" r:id="rId37" name="Control 51">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>25</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>25</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2099" r:id="rId37" name="Control 51"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2098" r:id="rId38" name="Control 50">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>24</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>24</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2098" r:id="rId38" name="Control 50"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2097" r:id="rId39" name="Control 49">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>24</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>24</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2097" r:id="rId39" name="Control 49"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2096" r:id="rId40" name="Control 48">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>23</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>23</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2096" r:id="rId40" name="Control 48"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2095" r:id="rId41" name="Control 47">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>23</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>23</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2095" r:id="rId41" name="Control 47"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2094" r:id="rId42" name="Control 46">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>22</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>22</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2094" r:id="rId42" name="Control 46"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2093" r:id="rId43" name="Control 45">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>22</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>22</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2093" r:id="rId43" name="Control 45"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2092" r:id="rId44" name="Control 44">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>21</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>21</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2092" r:id="rId44" name="Control 44"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2091" r:id="rId45" name="Control 43">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>21</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>21</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2091" r:id="rId45" name="Control 43"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2090" r:id="rId46" name="Control 42">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>20</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>20</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2090" r:id="rId46" name="Control 42"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2089" r:id="rId47" name="Control 41">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>20</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>20</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2089" r:id="rId47" name="Control 41"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2088" r:id="rId48" name="Control 40">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>19</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>19</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2088" r:id="rId48" name="Control 40"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2087" r:id="rId49" name="Control 39">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>19</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>19</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2087" r:id="rId49" name="Control 39"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2086" r:id="rId50" name="Control 38">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>18</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>18</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2086" r:id="rId50" name="Control 38"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2085" r:id="rId51" name="Control 37">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>18</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>18</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2085" r:id="rId51" name="Control 37"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2084" r:id="rId52" name="Control 36">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>17</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>17</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2084" r:id="rId52" name="Control 36"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2083" r:id="rId53" name="Control 35">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>17</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>17</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2083" r:id="rId53" name="Control 35"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2082" r:id="rId54" name="Control 34">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>16</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>16</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2082" r:id="rId54" name="Control 34"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2081" r:id="rId55" name="Control 33">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>16</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>16</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2081" r:id="rId55" name="Control 33"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2080" r:id="rId56" name="Control 32">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>15</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>15</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2080" r:id="rId56" name="Control 32"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2079" r:id="rId57" name="Control 31">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>15</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>15</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2079" r:id="rId57" name="Control 31"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2078" r:id="rId58" name="Control 30">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>14</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>14</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2078" r:id="rId58" name="Control 30"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2077" r:id="rId59" name="Control 29">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>14</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>14</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2077" r:id="rId59" name="Control 29"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2076" r:id="rId60" name="Control 28">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>13</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>13</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2076" r:id="rId60" name="Control 28"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2075" r:id="rId61" name="Control 27">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>13</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>13</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2075" r:id="rId61" name="Control 27"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2074" r:id="rId62" name="Control 26">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2074" r:id="rId62" name="Control 26"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2073" r:id="rId63" name="Control 25">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2073" r:id="rId63" name="Control 25"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2072" r:id="rId64" name="Control 24">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>11</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>11</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2072" r:id="rId64" name="Control 24"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2071" r:id="rId65" name="Control 23">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>11</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>11</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2071" r:id="rId65" name="Control 23"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2070" r:id="rId66" name="Control 22">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2070" r:id="rId66" name="Control 22"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2069" r:id="rId67" name="Control 21">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2069" r:id="rId67" name="Control 21"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2068" r:id="rId68" name="Control 20">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>9</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>9</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2068" r:id="rId68" name="Control 20"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2067" r:id="rId69" name="Control 19">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>9</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>9</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2067" r:id="rId69" name="Control 19"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2066" r:id="rId70" name="Control 18">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2066" r:id="rId70" name="Control 18"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2065" r:id="rId71" name="Control 17">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2065" r:id="rId71" name="Control 17"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2064" r:id="rId72" name="Control 16">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2064" r:id="rId72" name="Control 16"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2063" r:id="rId73" name="Control 15">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2063" r:id="rId73" name="Control 15"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2062" r:id="rId74" name="Control 14">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2062" r:id="rId74" name="Control 14"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2061" r:id="rId75" name="Control 13">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2061" r:id="rId75" name="Control 13"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2060" r:id="rId76" name="Control 12">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2060" r:id="rId76" name="Control 12"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2059" r:id="rId77" name="Control 11">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2059" r:id="rId77" name="Control 11"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2058" r:id="rId78" name="Control 10">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2058" r:id="rId78" name="Control 10"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2057" r:id="rId79" name="Control 9">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2057" r:id="rId79" name="Control 9"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2056" r:id="rId80" name="Control 8">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2056" r:id="rId80" name="Control 8"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2055" r:id="rId81" name="Control 7">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2055" r:id="rId81" name="Control 7"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2054" r:id="rId82" name="Control 6">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2054" r:id="rId82" name="Control 6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2053" r:id="rId83" name="Control 5">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2053" r:id="rId83" name="Control 5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2052" r:id="rId84" name="Control 4">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2052" r:id="rId84" name="Control 4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2051" r:id="rId85" name="Control 3">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2051" r:id="rId85" name="Control 3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2050" r:id="rId86" name="Control 2">
           <controlPr defaultSize="0" r:id="rId4">
             <anchor moveWithCells="1">
               <from>
@@ -8771,12 +10869,12 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2049" r:id="rId3" name="Control 1"/>
+        <control shapeId="2050" r:id="rId86" name="Control 2"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2050" r:id="rId5" name="Control 2">
+        <control shapeId="2049" r:id="rId87" name="Control 1">
           <controlPr defaultSize="0" r:id="rId4">
             <anchor moveWithCells="1">
               <from>
@@ -8796,2057 +10894,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2050" r:id="rId5" name="Control 2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2051" r:id="rId6" name="Control 3">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2051" r:id="rId6" name="Control 3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2052" r:id="rId7" name="Control 4">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2052" r:id="rId7" name="Control 4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2053" r:id="rId8" name="Control 5">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2053" r:id="rId8" name="Control 5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2054" r:id="rId9" name="Control 6">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2054" r:id="rId9" name="Control 6"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2055" r:id="rId10" name="Control 7">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2055" r:id="rId10" name="Control 7"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2056" r:id="rId11" name="Control 8">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2056" r:id="rId11" name="Control 8"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2057" r:id="rId12" name="Control 9">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2057" r:id="rId12" name="Control 9"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2058" r:id="rId13" name="Control 10">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2058" r:id="rId13" name="Control 10"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2059" r:id="rId14" name="Control 11">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2059" r:id="rId14" name="Control 11"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2060" r:id="rId15" name="Control 12">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2060" r:id="rId15" name="Control 12"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2061" r:id="rId16" name="Control 13">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2061" r:id="rId16" name="Control 13"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2062" r:id="rId17" name="Control 14">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2062" r:id="rId17" name="Control 14"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2063" r:id="rId18" name="Control 15">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2063" r:id="rId18" name="Control 15"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2064" r:id="rId19" name="Control 16">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2064" r:id="rId19" name="Control 16"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2065" r:id="rId20" name="Control 17">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2065" r:id="rId20" name="Control 17"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2066" r:id="rId21" name="Control 18">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2066" r:id="rId21" name="Control 18"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2067" r:id="rId22" name="Control 19">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>9</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>9</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2067" r:id="rId22" name="Control 19"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2068" r:id="rId23" name="Control 20">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>9</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>9</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2068" r:id="rId23" name="Control 20"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2069" r:id="rId24" name="Control 21">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2069" r:id="rId24" name="Control 21"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2070" r:id="rId25" name="Control 22">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2070" r:id="rId25" name="Control 22"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2071" r:id="rId26" name="Control 23">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>11</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>11</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2071" r:id="rId26" name="Control 23"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2072" r:id="rId27" name="Control 24">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>11</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>11</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2072" r:id="rId27" name="Control 24"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2073" r:id="rId28" name="Control 25">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>12</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>12</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2073" r:id="rId28" name="Control 25"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2074" r:id="rId29" name="Control 26">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>12</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>12</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2074" r:id="rId29" name="Control 26"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2075" r:id="rId30" name="Control 27">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>13</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>13</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2075" r:id="rId30" name="Control 27"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2076" r:id="rId31" name="Control 28">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>13</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>13</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2076" r:id="rId31" name="Control 28"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2077" r:id="rId32" name="Control 29">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>14</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>14</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2077" r:id="rId32" name="Control 29"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2078" r:id="rId33" name="Control 30">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>14</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>14</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2078" r:id="rId33" name="Control 30"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2079" r:id="rId34" name="Control 31">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>15</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>15</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2079" r:id="rId34" name="Control 31"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2080" r:id="rId35" name="Control 32">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>15</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>15</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2080" r:id="rId35" name="Control 32"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2081" r:id="rId36" name="Control 33">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>16</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>16</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2081" r:id="rId36" name="Control 33"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2082" r:id="rId37" name="Control 34">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>16</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>16</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2082" r:id="rId37" name="Control 34"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2083" r:id="rId38" name="Control 35">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>17</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>17</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2083" r:id="rId38" name="Control 35"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2084" r:id="rId39" name="Control 36">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>17</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>17</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2084" r:id="rId39" name="Control 36"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2085" r:id="rId40" name="Control 37">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>18</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>18</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2085" r:id="rId40" name="Control 37"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2086" r:id="rId41" name="Control 38">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>18</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>18</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2086" r:id="rId41" name="Control 38"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2087" r:id="rId42" name="Control 39">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>19</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>19</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2087" r:id="rId42" name="Control 39"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2088" r:id="rId43" name="Control 40">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>19</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>19</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2088" r:id="rId43" name="Control 40"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2089" r:id="rId44" name="Control 41">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>20</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>20</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2089" r:id="rId44" name="Control 41"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2090" r:id="rId45" name="Control 42">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>20</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>20</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2090" r:id="rId45" name="Control 42"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2091" r:id="rId46" name="Control 43">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>21</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>21</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2091" r:id="rId46" name="Control 43"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2092" r:id="rId47" name="Control 44">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>21</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>21</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2092" r:id="rId47" name="Control 44"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2093" r:id="rId48" name="Control 45">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>22</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>22</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2093" r:id="rId48" name="Control 45"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2094" r:id="rId49" name="Control 46">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>22</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>22</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2094" r:id="rId49" name="Control 46"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2095" r:id="rId50" name="Control 47">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>23</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>23</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2095" r:id="rId50" name="Control 47"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2096" r:id="rId51" name="Control 48">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>23</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>23</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2096" r:id="rId51" name="Control 48"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2097" r:id="rId52" name="Control 49">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>24</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>24</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2097" r:id="rId52" name="Control 49"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2098" r:id="rId53" name="Control 50">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>24</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>24</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2098" r:id="rId53" name="Control 50"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2099" r:id="rId54" name="Control 51">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>25</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>25</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2099" r:id="rId54" name="Control 51"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2100" r:id="rId55" name="Control 52">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>25</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>25</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2100" r:id="rId55" name="Control 52"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2101" r:id="rId56" name="Control 53">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>26</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>26</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2101" r:id="rId56" name="Control 53"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2102" r:id="rId57" name="Control 54">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>26</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>26</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2102" r:id="rId57" name="Control 54"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2103" r:id="rId58" name="Control 55">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>27</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>27</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2103" r:id="rId58" name="Control 55"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2104" r:id="rId59" name="Control 56">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>27</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>27</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2104" r:id="rId59" name="Control 56"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2105" r:id="rId60" name="Control 57">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>28</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>28</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2105" r:id="rId60" name="Control 57"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2106" r:id="rId61" name="Control 58">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>28</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>28</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2106" r:id="rId61" name="Control 58"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2107" r:id="rId62" name="Control 59">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>29</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>29</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2107" r:id="rId62" name="Control 59"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2108" r:id="rId63" name="Control 60">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>29</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>29</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2108" r:id="rId63" name="Control 60"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2109" r:id="rId64" name="Control 61">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>30</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>30</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2109" r:id="rId64" name="Control 61"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2110" r:id="rId65" name="Control 62">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>30</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>30</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2110" r:id="rId65" name="Control 62"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2111" r:id="rId66" name="Control 63">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>31</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>31</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2111" r:id="rId66" name="Control 63"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2112" r:id="rId67" name="Control 64">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>31</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>31</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2112" r:id="rId67" name="Control 64"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2113" r:id="rId68" name="Control 65">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>32</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>32</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2113" r:id="rId68" name="Control 65"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2114" r:id="rId69" name="Control 66">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>32</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>32</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2114" r:id="rId69" name="Control 66"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2115" r:id="rId70" name="Control 67">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>33</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>33</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2115" r:id="rId70" name="Control 67"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2116" r:id="rId71" name="Control 68">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>33</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>33</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2116" r:id="rId71" name="Control 68"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2117" r:id="rId72" name="Control 69">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>34</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>34</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2117" r:id="rId72" name="Control 69"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2118" r:id="rId73" name="Control 70">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>34</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>34</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2118" r:id="rId73" name="Control 70"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2119" r:id="rId74" name="Control 71">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>35</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>35</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2119" r:id="rId74" name="Control 71"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2120" r:id="rId75" name="Control 72">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>35</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>35</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2120" r:id="rId75" name="Control 72"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2121" r:id="rId76" name="Control 73">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>36</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>36</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2121" r:id="rId76" name="Control 73"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2122" r:id="rId77" name="Control 74">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>36</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>36</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2122" r:id="rId77" name="Control 74"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2123" r:id="rId78" name="Control 75">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>37</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>37</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2123" r:id="rId78" name="Control 75"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2124" r:id="rId79" name="Control 76">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>37</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>37</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2124" r:id="rId79" name="Control 76"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2125" r:id="rId80" name="Control 77">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>38</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>38</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2125" r:id="rId80" name="Control 77"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2126" r:id="rId81" name="Control 78">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>38</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>38</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2126" r:id="rId81" name="Control 78"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2127" r:id="rId82" name="Control 79">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>39</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>39</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2127" r:id="rId82" name="Control 79"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2128" r:id="rId83" name="Control 80">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>39</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>39</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2128" r:id="rId83" name="Control 80"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2129" r:id="rId84" name="Control 81">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>40</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>40</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2129" r:id="rId84" name="Control 81"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2130" r:id="rId85" name="Control 82">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>40</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>40</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2130" r:id="rId85" name="Control 82"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2131" r:id="rId86" name="Control 83">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>41</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>41</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2131" r:id="rId86" name="Control 83"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2132" r:id="rId87" name="Control 84">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>41</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>41</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2132" r:id="rId87" name="Control 84"/>
+        <control shapeId="2049" r:id="rId87" name="Control 1"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>

<commit_message>
update current sense resistor to 100m ohm from 560m ohm
</commit_message>
<xml_diff>
--- a/AxxSolder_hardware/bom/BOM_AxxSolder_V3_0.xlsx
+++ b/AxxSolder_hardware/bom/BOM_AxxSolder_V3_0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\axelj\ownCloud\2_Project\00_AxxProjects\AxxSolder\AxxSolder_hardware\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A1FC4CF-7B49-481D-B329-DECB60D1F996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{062614C8-55B4-4A3C-A136-3E44360BAA72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{60354D9D-8798-4211-B1E3-D5485177CC9B}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="248">
   <si>
     <t>References</t>
   </si>
@@ -762,6 +762,15 @@
   </si>
   <si>
     <t>0154007.DR</t>
+  </si>
+  <si>
+    <t>100m</t>
+  </si>
+  <si>
+    <t>ERJ-6DSFR10V</t>
+  </si>
+  <si>
+    <t>667-ERJ-6DSFR10V</t>
   </si>
 </sst>
 </file>
@@ -769,10 +778,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="164" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="#,##0.00\ [$€-1];[Red]\-#,##0.00\ [$€-1]"/>
-    <numFmt numFmtId="166" formatCode="_-* #,##0.00\ [$€-1]_-;\-* #,##0.00\ [$€-1]_-;_-* &quot;-&quot;??\ [$€-1]_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="165" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="#,##0.00\ [$€-1];[Red]\-#,##0.00\ [$€-1]"/>
+    <numFmt numFmtId="167" formatCode="_-* #,##0.00\ [$€-1]_-;\-* #,##0.00\ [$€-1]_-;_-* &quot;-&quot;??\ [$€-1]_-;_-@_-"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -952,12 +961,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="8" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -966,23 +975,23 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -5869,8 +5878,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:M79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6310,7 +6319,7 @@
         <v>187</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>188</v>
+        <v>245</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>186</v>
@@ -6319,20 +6328,20 @@
         <v>18</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>211</v>
+        <v>246</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>212</v>
+        <v>247</v>
       </c>
       <c r="G16" s="1">
         <v>1</v>
       </c>
       <c r="H16" s="15">
-        <v>0.36299999999999999</v>
+        <v>0.40899999999999997</v>
       </c>
       <c r="I16" s="15">
         <f t="shared" si="0"/>
-        <v>0.36299999999999999</v>
+        <v>0.40899999999999997</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7220,7 +7229,7 @@
       <c r="F46" s="7"/>
       <c r="I46" s="8">
         <f>SUM(I4:I45)</f>
-        <v>74.927000000000007</v>
+        <v>74.972999999999999</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
@@ -7643,7 +7652,7 @@
       <c r="E78" s="11"/>
       <c r="F78" s="20">
         <f>F76+G65+I46+G68</f>
-        <v>394.702</v>
+        <v>394.74800000000005</v>
       </c>
       <c r="G78" s="20"/>
     </row>
@@ -7657,7 +7666,7 @@
       <c r="E79" s="11"/>
       <c r="F79" s="20">
         <f>F76+G65+I46+G71</f>
-        <v>258.36200000000002</v>
+        <v>258.40800000000002</v>
       </c>
       <c r="G79" s="20"/>
     </row>
@@ -8799,7 +8808,2057 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2049" r:id="rId3" name="Control 1">
+        <control shapeId="2132" r:id="rId3" name="Control 84">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>41</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>41</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2132" r:id="rId3" name="Control 84"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2131" r:id="rId5" name="Control 83">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>41</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>41</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2131" r:id="rId5" name="Control 83"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2130" r:id="rId6" name="Control 82">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>40</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>40</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2130" r:id="rId6" name="Control 82"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2129" r:id="rId7" name="Control 81">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>40</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>40</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2129" r:id="rId7" name="Control 81"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2128" r:id="rId8" name="Control 80">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>39</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>39</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2128" r:id="rId8" name="Control 80"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2127" r:id="rId9" name="Control 79">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>39</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>39</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2127" r:id="rId9" name="Control 79"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2126" r:id="rId10" name="Control 78">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>38</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>38</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2126" r:id="rId10" name="Control 78"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2125" r:id="rId11" name="Control 77">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>38</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>38</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2125" r:id="rId11" name="Control 77"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2124" r:id="rId12" name="Control 76">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>37</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>37</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2124" r:id="rId12" name="Control 76"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2123" r:id="rId13" name="Control 75">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>37</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>37</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2123" r:id="rId13" name="Control 75"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2122" r:id="rId14" name="Control 74">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>36</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>36</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2122" r:id="rId14" name="Control 74"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2121" r:id="rId15" name="Control 73">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>36</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>36</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2121" r:id="rId15" name="Control 73"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2120" r:id="rId16" name="Control 72">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>35</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>35</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2120" r:id="rId16" name="Control 72"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2119" r:id="rId17" name="Control 71">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>35</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>35</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2119" r:id="rId17" name="Control 71"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2118" r:id="rId18" name="Control 70">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>34</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>34</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2118" r:id="rId18" name="Control 70"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2117" r:id="rId19" name="Control 69">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>34</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>34</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2117" r:id="rId19" name="Control 69"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2116" r:id="rId20" name="Control 68">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>33</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>33</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2116" r:id="rId20" name="Control 68"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2115" r:id="rId21" name="Control 67">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>33</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>33</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2115" r:id="rId21" name="Control 67"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2114" r:id="rId22" name="Control 66">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>32</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>32</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2114" r:id="rId22" name="Control 66"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2113" r:id="rId23" name="Control 65">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>32</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>32</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2113" r:id="rId23" name="Control 65"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2112" r:id="rId24" name="Control 64">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>31</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>31</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2112" r:id="rId24" name="Control 64"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2111" r:id="rId25" name="Control 63">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>31</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>31</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2111" r:id="rId25" name="Control 63"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2110" r:id="rId26" name="Control 62">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>30</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>30</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2110" r:id="rId26" name="Control 62"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2109" r:id="rId27" name="Control 61">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>30</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>30</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2109" r:id="rId27" name="Control 61"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2108" r:id="rId28" name="Control 60">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>29</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>29</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2108" r:id="rId28" name="Control 60"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2107" r:id="rId29" name="Control 59">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>29</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>29</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2107" r:id="rId29" name="Control 59"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2106" r:id="rId30" name="Control 58">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>28</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>28</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2106" r:id="rId30" name="Control 58"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2105" r:id="rId31" name="Control 57">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>28</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>28</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2105" r:id="rId31" name="Control 57"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2104" r:id="rId32" name="Control 56">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>27</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>27</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2104" r:id="rId32" name="Control 56"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2103" r:id="rId33" name="Control 55">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>27</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>27</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2103" r:id="rId33" name="Control 55"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2102" r:id="rId34" name="Control 54">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>26</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>26</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2102" r:id="rId34" name="Control 54"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2101" r:id="rId35" name="Control 53">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>26</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>26</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2101" r:id="rId35" name="Control 53"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2100" r:id="rId36" name="Control 52">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>25</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>25</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2100" r:id="rId36" name="Control 52"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2099" r:id="rId37" name="Control 51">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>25</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>25</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2099" r:id="rId37" name="Control 51"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2098" r:id="rId38" name="Control 50">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>24</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>24</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2098" r:id="rId38" name="Control 50"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2097" r:id="rId39" name="Control 49">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>24</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>24</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2097" r:id="rId39" name="Control 49"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2096" r:id="rId40" name="Control 48">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>23</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>23</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2096" r:id="rId40" name="Control 48"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2095" r:id="rId41" name="Control 47">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>23</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>23</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2095" r:id="rId41" name="Control 47"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2094" r:id="rId42" name="Control 46">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>22</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>22</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2094" r:id="rId42" name="Control 46"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2093" r:id="rId43" name="Control 45">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>22</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>22</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2093" r:id="rId43" name="Control 45"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2092" r:id="rId44" name="Control 44">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>21</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>21</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2092" r:id="rId44" name="Control 44"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2091" r:id="rId45" name="Control 43">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>21</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>21</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2091" r:id="rId45" name="Control 43"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2090" r:id="rId46" name="Control 42">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>20</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>20</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2090" r:id="rId46" name="Control 42"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2089" r:id="rId47" name="Control 41">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>20</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>20</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2089" r:id="rId47" name="Control 41"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2088" r:id="rId48" name="Control 40">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>19</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>19</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2088" r:id="rId48" name="Control 40"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2087" r:id="rId49" name="Control 39">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>19</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>19</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2087" r:id="rId49" name="Control 39"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2086" r:id="rId50" name="Control 38">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>18</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>18</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2086" r:id="rId50" name="Control 38"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2085" r:id="rId51" name="Control 37">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>18</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>18</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2085" r:id="rId51" name="Control 37"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2084" r:id="rId52" name="Control 36">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>17</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>17</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2084" r:id="rId52" name="Control 36"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2083" r:id="rId53" name="Control 35">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>17</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>17</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2083" r:id="rId53" name="Control 35"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2082" r:id="rId54" name="Control 34">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>16</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>16</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2082" r:id="rId54" name="Control 34"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2081" r:id="rId55" name="Control 33">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>16</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>16</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2081" r:id="rId55" name="Control 33"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2080" r:id="rId56" name="Control 32">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>15</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>15</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2080" r:id="rId56" name="Control 32"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2079" r:id="rId57" name="Control 31">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>15</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>15</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2079" r:id="rId57" name="Control 31"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2078" r:id="rId58" name="Control 30">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>14</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>14</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2078" r:id="rId58" name="Control 30"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2077" r:id="rId59" name="Control 29">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>14</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>14</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2077" r:id="rId59" name="Control 29"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2076" r:id="rId60" name="Control 28">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>13</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>13</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2076" r:id="rId60" name="Control 28"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2075" r:id="rId61" name="Control 27">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>13</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>13</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2075" r:id="rId61" name="Control 27"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2074" r:id="rId62" name="Control 26">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2074" r:id="rId62" name="Control 26"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2073" r:id="rId63" name="Control 25">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2073" r:id="rId63" name="Control 25"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2072" r:id="rId64" name="Control 24">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>11</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>11</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2072" r:id="rId64" name="Control 24"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2071" r:id="rId65" name="Control 23">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>11</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>11</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2071" r:id="rId65" name="Control 23"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2070" r:id="rId66" name="Control 22">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2070" r:id="rId66" name="Control 22"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2069" r:id="rId67" name="Control 21">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2069" r:id="rId67" name="Control 21"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2068" r:id="rId68" name="Control 20">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>9</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>9</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2068" r:id="rId68" name="Control 20"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2067" r:id="rId69" name="Control 19">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>9</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>9</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2067" r:id="rId69" name="Control 19"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2066" r:id="rId70" name="Control 18">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2066" r:id="rId70" name="Control 18"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2065" r:id="rId71" name="Control 17">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2065" r:id="rId71" name="Control 17"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2064" r:id="rId72" name="Control 16">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2064" r:id="rId72" name="Control 16"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2063" r:id="rId73" name="Control 15">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2063" r:id="rId73" name="Control 15"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2062" r:id="rId74" name="Control 14">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2062" r:id="rId74" name="Control 14"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2061" r:id="rId75" name="Control 13">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2061" r:id="rId75" name="Control 13"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2060" r:id="rId76" name="Control 12">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2060" r:id="rId76" name="Control 12"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2059" r:id="rId77" name="Control 11">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2059" r:id="rId77" name="Control 11"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2058" r:id="rId78" name="Control 10">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2058" r:id="rId78" name="Control 10"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2057" r:id="rId79" name="Control 9">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2057" r:id="rId79" name="Control 9"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2056" r:id="rId80" name="Control 8">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2056" r:id="rId80" name="Control 8"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2055" r:id="rId81" name="Control 7">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2055" r:id="rId81" name="Control 7"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2054" r:id="rId82" name="Control 6">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2054" r:id="rId82" name="Control 6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2053" r:id="rId83" name="Control 5">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2053" r:id="rId83" name="Control 5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2052" r:id="rId84" name="Control 4">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2052" r:id="rId84" name="Control 4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2051" r:id="rId85" name="Control 3">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2051" r:id="rId85" name="Control 3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2050" r:id="rId86" name="Control 2">
           <controlPr defaultSize="0" r:id="rId4">
             <anchor moveWithCells="1">
               <from>
@@ -8819,12 +10878,12 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2049" r:id="rId3" name="Control 1"/>
+        <control shapeId="2050" r:id="rId86" name="Control 2"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2050" r:id="rId5" name="Control 2">
+        <control shapeId="2049" r:id="rId87" name="Control 1">
           <controlPr defaultSize="0" r:id="rId4">
             <anchor moveWithCells="1">
               <from>
@@ -8844,2057 +10903,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2050" r:id="rId5" name="Control 2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2051" r:id="rId6" name="Control 3">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2051" r:id="rId6" name="Control 3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2052" r:id="rId7" name="Control 4">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2052" r:id="rId7" name="Control 4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2053" r:id="rId8" name="Control 5">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2053" r:id="rId8" name="Control 5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2054" r:id="rId9" name="Control 6">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2054" r:id="rId9" name="Control 6"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2055" r:id="rId10" name="Control 7">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2055" r:id="rId10" name="Control 7"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2056" r:id="rId11" name="Control 8">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2056" r:id="rId11" name="Control 8"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2057" r:id="rId12" name="Control 9">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2057" r:id="rId12" name="Control 9"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2058" r:id="rId13" name="Control 10">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2058" r:id="rId13" name="Control 10"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2059" r:id="rId14" name="Control 11">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2059" r:id="rId14" name="Control 11"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2060" r:id="rId15" name="Control 12">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2060" r:id="rId15" name="Control 12"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2061" r:id="rId16" name="Control 13">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2061" r:id="rId16" name="Control 13"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2062" r:id="rId17" name="Control 14">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2062" r:id="rId17" name="Control 14"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2063" r:id="rId18" name="Control 15">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2063" r:id="rId18" name="Control 15"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2064" r:id="rId19" name="Control 16">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2064" r:id="rId19" name="Control 16"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2065" r:id="rId20" name="Control 17">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2065" r:id="rId20" name="Control 17"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2066" r:id="rId21" name="Control 18">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2066" r:id="rId21" name="Control 18"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2067" r:id="rId22" name="Control 19">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>9</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>9</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2067" r:id="rId22" name="Control 19"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2068" r:id="rId23" name="Control 20">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>9</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>9</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2068" r:id="rId23" name="Control 20"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2069" r:id="rId24" name="Control 21">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2069" r:id="rId24" name="Control 21"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2070" r:id="rId25" name="Control 22">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2070" r:id="rId25" name="Control 22"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2071" r:id="rId26" name="Control 23">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>11</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>11</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2071" r:id="rId26" name="Control 23"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2072" r:id="rId27" name="Control 24">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>11</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>11</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2072" r:id="rId27" name="Control 24"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2073" r:id="rId28" name="Control 25">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>12</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>12</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2073" r:id="rId28" name="Control 25"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2074" r:id="rId29" name="Control 26">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>12</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>12</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2074" r:id="rId29" name="Control 26"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2075" r:id="rId30" name="Control 27">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>13</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>13</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2075" r:id="rId30" name="Control 27"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2076" r:id="rId31" name="Control 28">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>13</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>13</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2076" r:id="rId31" name="Control 28"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2077" r:id="rId32" name="Control 29">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>14</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>14</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2077" r:id="rId32" name="Control 29"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2078" r:id="rId33" name="Control 30">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>14</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>14</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2078" r:id="rId33" name="Control 30"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2079" r:id="rId34" name="Control 31">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>15</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>15</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2079" r:id="rId34" name="Control 31"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2080" r:id="rId35" name="Control 32">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>15</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>15</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2080" r:id="rId35" name="Control 32"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2081" r:id="rId36" name="Control 33">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>16</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>16</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2081" r:id="rId36" name="Control 33"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2082" r:id="rId37" name="Control 34">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>16</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>16</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2082" r:id="rId37" name="Control 34"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2083" r:id="rId38" name="Control 35">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>17</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>17</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2083" r:id="rId38" name="Control 35"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2084" r:id="rId39" name="Control 36">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>17</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>17</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2084" r:id="rId39" name="Control 36"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2085" r:id="rId40" name="Control 37">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>18</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>18</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2085" r:id="rId40" name="Control 37"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2086" r:id="rId41" name="Control 38">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>18</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>18</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2086" r:id="rId41" name="Control 38"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2087" r:id="rId42" name="Control 39">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>19</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>19</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2087" r:id="rId42" name="Control 39"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2088" r:id="rId43" name="Control 40">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>19</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>19</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2088" r:id="rId43" name="Control 40"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2089" r:id="rId44" name="Control 41">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>20</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>20</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2089" r:id="rId44" name="Control 41"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2090" r:id="rId45" name="Control 42">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>20</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>20</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2090" r:id="rId45" name="Control 42"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2091" r:id="rId46" name="Control 43">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>21</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>21</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2091" r:id="rId46" name="Control 43"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2092" r:id="rId47" name="Control 44">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>21</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>21</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2092" r:id="rId47" name="Control 44"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2093" r:id="rId48" name="Control 45">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>22</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>22</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2093" r:id="rId48" name="Control 45"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2094" r:id="rId49" name="Control 46">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>22</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>22</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2094" r:id="rId49" name="Control 46"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2095" r:id="rId50" name="Control 47">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>23</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>23</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2095" r:id="rId50" name="Control 47"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2096" r:id="rId51" name="Control 48">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>23</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>23</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2096" r:id="rId51" name="Control 48"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2097" r:id="rId52" name="Control 49">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>24</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>24</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2097" r:id="rId52" name="Control 49"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2098" r:id="rId53" name="Control 50">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>24</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>24</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2098" r:id="rId53" name="Control 50"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2099" r:id="rId54" name="Control 51">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>25</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>25</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2099" r:id="rId54" name="Control 51"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2100" r:id="rId55" name="Control 52">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>25</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>25</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2100" r:id="rId55" name="Control 52"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2101" r:id="rId56" name="Control 53">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>26</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>26</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2101" r:id="rId56" name="Control 53"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2102" r:id="rId57" name="Control 54">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>26</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>26</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2102" r:id="rId57" name="Control 54"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2103" r:id="rId58" name="Control 55">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>27</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>27</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2103" r:id="rId58" name="Control 55"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2104" r:id="rId59" name="Control 56">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>27</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>27</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2104" r:id="rId59" name="Control 56"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2105" r:id="rId60" name="Control 57">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>28</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>28</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2105" r:id="rId60" name="Control 57"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2106" r:id="rId61" name="Control 58">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>28</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>28</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2106" r:id="rId61" name="Control 58"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2107" r:id="rId62" name="Control 59">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>29</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>29</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2107" r:id="rId62" name="Control 59"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2108" r:id="rId63" name="Control 60">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>29</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>29</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2108" r:id="rId63" name="Control 60"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2109" r:id="rId64" name="Control 61">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>30</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>30</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2109" r:id="rId64" name="Control 61"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2110" r:id="rId65" name="Control 62">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>30</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>30</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2110" r:id="rId65" name="Control 62"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2111" r:id="rId66" name="Control 63">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>31</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>31</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2111" r:id="rId66" name="Control 63"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2112" r:id="rId67" name="Control 64">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>31</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>31</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2112" r:id="rId67" name="Control 64"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2113" r:id="rId68" name="Control 65">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>32</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>32</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2113" r:id="rId68" name="Control 65"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2114" r:id="rId69" name="Control 66">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>32</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>32</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2114" r:id="rId69" name="Control 66"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2115" r:id="rId70" name="Control 67">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>33</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>33</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2115" r:id="rId70" name="Control 67"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2116" r:id="rId71" name="Control 68">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>33</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>33</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2116" r:id="rId71" name="Control 68"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2117" r:id="rId72" name="Control 69">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>34</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>34</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2117" r:id="rId72" name="Control 69"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2118" r:id="rId73" name="Control 70">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>34</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>34</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2118" r:id="rId73" name="Control 70"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2119" r:id="rId74" name="Control 71">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>35</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>35</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2119" r:id="rId74" name="Control 71"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2120" r:id="rId75" name="Control 72">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>35</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>35</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2120" r:id="rId75" name="Control 72"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2121" r:id="rId76" name="Control 73">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>36</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>36</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2121" r:id="rId76" name="Control 73"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2122" r:id="rId77" name="Control 74">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>36</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>36</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2122" r:id="rId77" name="Control 74"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2123" r:id="rId78" name="Control 75">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>37</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>37</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2123" r:id="rId78" name="Control 75"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2124" r:id="rId79" name="Control 76">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>37</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>37</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2124" r:id="rId79" name="Control 76"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2125" r:id="rId80" name="Control 77">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>38</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>38</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2125" r:id="rId80" name="Control 77"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2126" r:id="rId81" name="Control 78">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>38</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>38</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2126" r:id="rId81" name="Control 78"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2127" r:id="rId82" name="Control 79">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>39</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>39</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2127" r:id="rId82" name="Control 79"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2128" r:id="rId83" name="Control 80">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>39</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>39</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2128" r:id="rId83" name="Control 80"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2129" r:id="rId84" name="Control 81">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>40</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>40</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2129" r:id="rId84" name="Control 81"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2130" r:id="rId85" name="Control 82">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>40</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>40</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2130" r:id="rId85" name="Control 82"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2131" r:id="rId86" name="Control 83">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>41</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>41</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2131" r:id="rId86" name="Control 83"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2132" r:id="rId87" name="Control 84">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>41</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>41</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2132" r:id="rId87" name="Control 84"/>
+        <control shapeId="2049" r:id="rId87" name="Control 1"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>

<commit_message>
Change IC9 from INA180 to INA281
</commit_message>
<xml_diff>
--- a/AxxSolder_hardware/bom/BOM_AxxSolder_V3_0.xlsx
+++ b/AxxSolder_hardware/bom/BOM_AxxSolder_V3_0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\axelj\ownCloud\2_Project\00_AxxProjects\AxxSolder\AxxSolder_hardware\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{062614C8-55B4-4A3C-A136-3E44360BAA72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3D266BB-5FE0-4472-8FA3-7D2258610F72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{60354D9D-8798-4211-B1E3-D5485177CC9B}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="250">
   <si>
     <t>References</t>
   </si>
@@ -771,6 +771,12 @@
   </si>
   <si>
     <t>667-ERJ-6DSFR10V</t>
+  </si>
+  <si>
+    <t>INA281A5QDBVRQ1</t>
+  </si>
+  <si>
+    <t>595-INA281A5QDBVRQ1</t>
   </si>
 </sst>
 </file>
@@ -5879,7 +5885,7 @@
   <dimension ref="A1:M79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6953,7 +6959,7 @@
         <v>201</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>202</v>
+        <v>248</v>
       </c>
       <c r="C37" s="12" t="s">
         <v>203</v>
@@ -6962,20 +6968,20 @@
         <v>91</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>202</v>
+        <v>248</v>
       </c>
       <c r="F37" s="12" t="s">
-        <v>219</v>
+        <v>249</v>
       </c>
       <c r="G37" s="12">
         <v>1</v>
       </c>
       <c r="H37" s="16">
-        <v>0.81799999999999995</v>
+        <v>2.74</v>
       </c>
       <c r="I37" s="15">
         <f t="shared" si="0"/>
-        <v>0.81799999999999995</v>
+        <v>2.74</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7229,7 +7235,7 @@
       <c r="F46" s="7"/>
       <c r="I46" s="8">
         <f>SUM(I4:I45)</f>
-        <v>74.972999999999999</v>
+        <v>76.894999999999996</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
@@ -7652,7 +7658,7 @@
       <c r="E78" s="11"/>
       <c r="F78" s="20">
         <f>F76+G65+I46+G68</f>
-        <v>394.74800000000005</v>
+        <v>396.66999999999996</v>
       </c>
       <c r="G78" s="20"/>
     </row>
@@ -7666,7 +7672,7 @@
       <c r="E79" s="11"/>
       <c r="F79" s="20">
         <f>F76+G65+I46+G71</f>
-        <v>258.40800000000002</v>
+        <v>260.33</v>
       </c>
       <c r="G79" s="20"/>
     </row>
@@ -8808,7 +8814,2057 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2132" r:id="rId3" name="Control 84">
+        <control shapeId="2049" r:id="rId3" name="Control 1">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2049" r:id="rId3" name="Control 1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2050" r:id="rId5" name="Control 2">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2050" r:id="rId5" name="Control 2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2051" r:id="rId6" name="Control 3">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2051" r:id="rId6" name="Control 3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2052" r:id="rId7" name="Control 4">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2052" r:id="rId7" name="Control 4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2053" r:id="rId8" name="Control 5">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2053" r:id="rId8" name="Control 5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2054" r:id="rId9" name="Control 6">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2054" r:id="rId9" name="Control 6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2055" r:id="rId10" name="Control 7">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2055" r:id="rId10" name="Control 7"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2056" r:id="rId11" name="Control 8">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2056" r:id="rId11" name="Control 8"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2057" r:id="rId12" name="Control 9">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2057" r:id="rId12" name="Control 9"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2058" r:id="rId13" name="Control 10">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2058" r:id="rId13" name="Control 10"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2059" r:id="rId14" name="Control 11">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2059" r:id="rId14" name="Control 11"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2060" r:id="rId15" name="Control 12">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2060" r:id="rId15" name="Control 12"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2061" r:id="rId16" name="Control 13">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2061" r:id="rId16" name="Control 13"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2062" r:id="rId17" name="Control 14">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2062" r:id="rId17" name="Control 14"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2063" r:id="rId18" name="Control 15">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2063" r:id="rId18" name="Control 15"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2064" r:id="rId19" name="Control 16">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2064" r:id="rId19" name="Control 16"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2065" r:id="rId20" name="Control 17">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2065" r:id="rId20" name="Control 17"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2066" r:id="rId21" name="Control 18">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2066" r:id="rId21" name="Control 18"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2067" r:id="rId22" name="Control 19">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>9</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>9</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2067" r:id="rId22" name="Control 19"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2068" r:id="rId23" name="Control 20">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>9</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>9</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2068" r:id="rId23" name="Control 20"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2069" r:id="rId24" name="Control 21">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2069" r:id="rId24" name="Control 21"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2070" r:id="rId25" name="Control 22">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2070" r:id="rId25" name="Control 22"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2071" r:id="rId26" name="Control 23">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>11</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>11</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2071" r:id="rId26" name="Control 23"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2072" r:id="rId27" name="Control 24">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>11</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>11</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2072" r:id="rId27" name="Control 24"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2073" r:id="rId28" name="Control 25">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2073" r:id="rId28" name="Control 25"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2074" r:id="rId29" name="Control 26">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2074" r:id="rId29" name="Control 26"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2075" r:id="rId30" name="Control 27">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>13</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>13</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2075" r:id="rId30" name="Control 27"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2076" r:id="rId31" name="Control 28">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>13</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>13</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2076" r:id="rId31" name="Control 28"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2077" r:id="rId32" name="Control 29">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>14</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>14</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2077" r:id="rId32" name="Control 29"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2078" r:id="rId33" name="Control 30">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>14</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>14</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2078" r:id="rId33" name="Control 30"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2079" r:id="rId34" name="Control 31">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>15</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>15</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2079" r:id="rId34" name="Control 31"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2080" r:id="rId35" name="Control 32">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>15</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>15</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2080" r:id="rId35" name="Control 32"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2081" r:id="rId36" name="Control 33">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>16</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>16</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2081" r:id="rId36" name="Control 33"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2082" r:id="rId37" name="Control 34">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>16</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>16</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2082" r:id="rId37" name="Control 34"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2083" r:id="rId38" name="Control 35">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>17</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>17</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2083" r:id="rId38" name="Control 35"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2084" r:id="rId39" name="Control 36">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>17</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>17</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2084" r:id="rId39" name="Control 36"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2085" r:id="rId40" name="Control 37">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>18</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>18</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2085" r:id="rId40" name="Control 37"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2086" r:id="rId41" name="Control 38">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>18</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>18</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2086" r:id="rId41" name="Control 38"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2087" r:id="rId42" name="Control 39">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>19</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>19</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2087" r:id="rId42" name="Control 39"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2088" r:id="rId43" name="Control 40">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>19</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>19</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2088" r:id="rId43" name="Control 40"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2089" r:id="rId44" name="Control 41">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>20</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>20</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2089" r:id="rId44" name="Control 41"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2090" r:id="rId45" name="Control 42">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>20</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>20</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2090" r:id="rId45" name="Control 42"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2091" r:id="rId46" name="Control 43">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>21</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>21</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2091" r:id="rId46" name="Control 43"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2092" r:id="rId47" name="Control 44">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>21</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>21</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2092" r:id="rId47" name="Control 44"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2093" r:id="rId48" name="Control 45">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>22</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>22</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2093" r:id="rId48" name="Control 45"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2094" r:id="rId49" name="Control 46">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>22</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>22</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2094" r:id="rId49" name="Control 46"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2095" r:id="rId50" name="Control 47">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>23</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>23</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2095" r:id="rId50" name="Control 47"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2096" r:id="rId51" name="Control 48">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>23</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>23</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2096" r:id="rId51" name="Control 48"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2097" r:id="rId52" name="Control 49">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>24</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>24</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2097" r:id="rId52" name="Control 49"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2098" r:id="rId53" name="Control 50">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>24</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>24</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2098" r:id="rId53" name="Control 50"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2099" r:id="rId54" name="Control 51">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>25</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>25</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2099" r:id="rId54" name="Control 51"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2100" r:id="rId55" name="Control 52">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>25</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>25</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2100" r:id="rId55" name="Control 52"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2101" r:id="rId56" name="Control 53">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>26</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>26</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2101" r:id="rId56" name="Control 53"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2102" r:id="rId57" name="Control 54">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>26</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>26</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2102" r:id="rId57" name="Control 54"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2103" r:id="rId58" name="Control 55">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>27</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>27</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2103" r:id="rId58" name="Control 55"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2104" r:id="rId59" name="Control 56">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>27</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>27</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2104" r:id="rId59" name="Control 56"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2105" r:id="rId60" name="Control 57">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>28</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>28</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2105" r:id="rId60" name="Control 57"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2106" r:id="rId61" name="Control 58">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>28</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>28</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2106" r:id="rId61" name="Control 58"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2107" r:id="rId62" name="Control 59">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>29</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>29</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2107" r:id="rId62" name="Control 59"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2108" r:id="rId63" name="Control 60">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>29</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>29</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2108" r:id="rId63" name="Control 60"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2109" r:id="rId64" name="Control 61">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>30</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>30</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2109" r:id="rId64" name="Control 61"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2110" r:id="rId65" name="Control 62">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>30</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>30</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2110" r:id="rId65" name="Control 62"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2111" r:id="rId66" name="Control 63">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>31</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>31</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2111" r:id="rId66" name="Control 63"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2112" r:id="rId67" name="Control 64">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>31</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>31</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2112" r:id="rId67" name="Control 64"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2113" r:id="rId68" name="Control 65">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>32</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>32</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2113" r:id="rId68" name="Control 65"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2114" r:id="rId69" name="Control 66">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>32</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>32</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2114" r:id="rId69" name="Control 66"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2115" r:id="rId70" name="Control 67">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>33</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>33</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2115" r:id="rId70" name="Control 67"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2116" r:id="rId71" name="Control 68">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>33</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>33</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2116" r:id="rId71" name="Control 68"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2117" r:id="rId72" name="Control 69">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>34</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>34</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2117" r:id="rId72" name="Control 69"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2118" r:id="rId73" name="Control 70">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>34</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>34</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2118" r:id="rId73" name="Control 70"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2119" r:id="rId74" name="Control 71">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>35</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>35</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2119" r:id="rId74" name="Control 71"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2120" r:id="rId75" name="Control 72">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>35</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>35</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2120" r:id="rId75" name="Control 72"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2121" r:id="rId76" name="Control 73">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>36</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>36</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2121" r:id="rId76" name="Control 73"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2122" r:id="rId77" name="Control 74">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>36</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>36</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2122" r:id="rId77" name="Control 74"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2123" r:id="rId78" name="Control 75">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>37</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>37</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2123" r:id="rId78" name="Control 75"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2124" r:id="rId79" name="Control 76">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>37</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>37</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2124" r:id="rId79" name="Control 76"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2125" r:id="rId80" name="Control 77">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>38</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>38</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2125" r:id="rId80" name="Control 77"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2126" r:id="rId81" name="Control 78">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>38</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>38</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2126" r:id="rId81" name="Control 78"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2127" r:id="rId82" name="Control 79">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>39</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>39</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2127" r:id="rId82" name="Control 79"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2128" r:id="rId83" name="Control 80">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>39</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>39</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2128" r:id="rId83" name="Control 80"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2129" r:id="rId84" name="Control 81">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>40</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>40</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2129" r:id="rId84" name="Control 81"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2130" r:id="rId85" name="Control 82">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>40</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>40</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="2130" r:id="rId85" name="Control 82"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="2131" r:id="rId86" name="Control 83">
           <controlPr defaultSize="0" r:id="rId4">
             <anchor moveWithCells="1">
               <from>
@@ -8828,12 +10884,12 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2132" r:id="rId3" name="Control 84"/>
+        <control shapeId="2131" r:id="rId86" name="Control 83"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2131" r:id="rId5" name="Control 83">
+        <control shapeId="2132" r:id="rId87" name="Control 84">
           <controlPr defaultSize="0" r:id="rId4">
             <anchor moveWithCells="1">
               <from>
@@ -8853,2057 +10909,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2131" r:id="rId5" name="Control 83"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2130" r:id="rId6" name="Control 82">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>40</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>40</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2130" r:id="rId6" name="Control 82"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2129" r:id="rId7" name="Control 81">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>40</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>40</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2129" r:id="rId7" name="Control 81"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2128" r:id="rId8" name="Control 80">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>39</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>39</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2128" r:id="rId8" name="Control 80"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2127" r:id="rId9" name="Control 79">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>39</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>39</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2127" r:id="rId9" name="Control 79"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2126" r:id="rId10" name="Control 78">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>38</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>38</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2126" r:id="rId10" name="Control 78"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2125" r:id="rId11" name="Control 77">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>38</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>38</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2125" r:id="rId11" name="Control 77"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2124" r:id="rId12" name="Control 76">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>37</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>37</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2124" r:id="rId12" name="Control 76"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2123" r:id="rId13" name="Control 75">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>37</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>37</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2123" r:id="rId13" name="Control 75"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2122" r:id="rId14" name="Control 74">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>36</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>36</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2122" r:id="rId14" name="Control 74"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2121" r:id="rId15" name="Control 73">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>36</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>36</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2121" r:id="rId15" name="Control 73"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2120" r:id="rId16" name="Control 72">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>35</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>35</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2120" r:id="rId16" name="Control 72"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2119" r:id="rId17" name="Control 71">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>35</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>35</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2119" r:id="rId17" name="Control 71"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2118" r:id="rId18" name="Control 70">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>34</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>34</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2118" r:id="rId18" name="Control 70"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2117" r:id="rId19" name="Control 69">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>34</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>34</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2117" r:id="rId19" name="Control 69"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2116" r:id="rId20" name="Control 68">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>33</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>33</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2116" r:id="rId20" name="Control 68"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2115" r:id="rId21" name="Control 67">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>33</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>33</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2115" r:id="rId21" name="Control 67"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2114" r:id="rId22" name="Control 66">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>32</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>32</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2114" r:id="rId22" name="Control 66"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2113" r:id="rId23" name="Control 65">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>32</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>32</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2113" r:id="rId23" name="Control 65"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2112" r:id="rId24" name="Control 64">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>31</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>31</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2112" r:id="rId24" name="Control 64"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2111" r:id="rId25" name="Control 63">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>31</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>31</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2111" r:id="rId25" name="Control 63"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2110" r:id="rId26" name="Control 62">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>30</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>30</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2110" r:id="rId26" name="Control 62"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2109" r:id="rId27" name="Control 61">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>30</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>30</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2109" r:id="rId27" name="Control 61"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2108" r:id="rId28" name="Control 60">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>29</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>29</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2108" r:id="rId28" name="Control 60"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2107" r:id="rId29" name="Control 59">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>29</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>29</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2107" r:id="rId29" name="Control 59"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2106" r:id="rId30" name="Control 58">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>28</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>28</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2106" r:id="rId30" name="Control 58"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2105" r:id="rId31" name="Control 57">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>28</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>28</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2105" r:id="rId31" name="Control 57"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2104" r:id="rId32" name="Control 56">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>27</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>27</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2104" r:id="rId32" name="Control 56"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2103" r:id="rId33" name="Control 55">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>27</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>27</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2103" r:id="rId33" name="Control 55"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2102" r:id="rId34" name="Control 54">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>26</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>26</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2102" r:id="rId34" name="Control 54"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2101" r:id="rId35" name="Control 53">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>26</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>26</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2101" r:id="rId35" name="Control 53"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2100" r:id="rId36" name="Control 52">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>25</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>25</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2100" r:id="rId36" name="Control 52"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2099" r:id="rId37" name="Control 51">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>25</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>25</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2099" r:id="rId37" name="Control 51"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2098" r:id="rId38" name="Control 50">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>24</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>24</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2098" r:id="rId38" name="Control 50"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2097" r:id="rId39" name="Control 49">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>24</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>24</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2097" r:id="rId39" name="Control 49"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2096" r:id="rId40" name="Control 48">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>23</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>23</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2096" r:id="rId40" name="Control 48"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2095" r:id="rId41" name="Control 47">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>23</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>23</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2095" r:id="rId41" name="Control 47"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2094" r:id="rId42" name="Control 46">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>22</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>22</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2094" r:id="rId42" name="Control 46"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2093" r:id="rId43" name="Control 45">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>22</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>22</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2093" r:id="rId43" name="Control 45"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2092" r:id="rId44" name="Control 44">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>21</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>21</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2092" r:id="rId44" name="Control 44"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2091" r:id="rId45" name="Control 43">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>21</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>21</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2091" r:id="rId45" name="Control 43"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2090" r:id="rId46" name="Control 42">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>20</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>20</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2090" r:id="rId46" name="Control 42"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2089" r:id="rId47" name="Control 41">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>20</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>20</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2089" r:id="rId47" name="Control 41"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2088" r:id="rId48" name="Control 40">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>19</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>19</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2088" r:id="rId48" name="Control 40"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2087" r:id="rId49" name="Control 39">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>19</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>19</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2087" r:id="rId49" name="Control 39"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2086" r:id="rId50" name="Control 38">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>18</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>18</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2086" r:id="rId50" name="Control 38"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2085" r:id="rId51" name="Control 37">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>18</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>18</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2085" r:id="rId51" name="Control 37"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2084" r:id="rId52" name="Control 36">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>17</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>17</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2084" r:id="rId52" name="Control 36"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2083" r:id="rId53" name="Control 35">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>17</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>17</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2083" r:id="rId53" name="Control 35"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2082" r:id="rId54" name="Control 34">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>16</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>16</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2082" r:id="rId54" name="Control 34"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2081" r:id="rId55" name="Control 33">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>16</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>16</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2081" r:id="rId55" name="Control 33"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2080" r:id="rId56" name="Control 32">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>15</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>15</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2080" r:id="rId56" name="Control 32"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2079" r:id="rId57" name="Control 31">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>15</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>15</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2079" r:id="rId57" name="Control 31"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2078" r:id="rId58" name="Control 30">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>14</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>14</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2078" r:id="rId58" name="Control 30"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2077" r:id="rId59" name="Control 29">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>14</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>14</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2077" r:id="rId59" name="Control 29"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2076" r:id="rId60" name="Control 28">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>13</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>13</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2076" r:id="rId60" name="Control 28"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2075" r:id="rId61" name="Control 27">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>13</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>13</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2075" r:id="rId61" name="Control 27"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2074" r:id="rId62" name="Control 26">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>12</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>12</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2074" r:id="rId62" name="Control 26"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2073" r:id="rId63" name="Control 25">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>12</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>12</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2073" r:id="rId63" name="Control 25"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2072" r:id="rId64" name="Control 24">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>11</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>11</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2072" r:id="rId64" name="Control 24"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2071" r:id="rId65" name="Control 23">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>11</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>11</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2071" r:id="rId65" name="Control 23"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2070" r:id="rId66" name="Control 22">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2070" r:id="rId66" name="Control 22"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2069" r:id="rId67" name="Control 21">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2069" r:id="rId67" name="Control 21"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2068" r:id="rId68" name="Control 20">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>9</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>9</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2068" r:id="rId68" name="Control 20"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2067" r:id="rId69" name="Control 19">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>9</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>9</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2067" r:id="rId69" name="Control 19"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2066" r:id="rId70" name="Control 18">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2066" r:id="rId70" name="Control 18"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2065" r:id="rId71" name="Control 17">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2065" r:id="rId71" name="Control 17"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2064" r:id="rId72" name="Control 16">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2064" r:id="rId72" name="Control 16"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2063" r:id="rId73" name="Control 15">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2063" r:id="rId73" name="Control 15"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2062" r:id="rId74" name="Control 14">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2062" r:id="rId74" name="Control 14"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2061" r:id="rId75" name="Control 13">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2061" r:id="rId75" name="Control 13"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2060" r:id="rId76" name="Control 12">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2060" r:id="rId76" name="Control 12"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2059" r:id="rId77" name="Control 11">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2059" r:id="rId77" name="Control 11"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2058" r:id="rId78" name="Control 10">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2058" r:id="rId78" name="Control 10"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2057" r:id="rId79" name="Control 9">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2057" r:id="rId79" name="Control 9"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2056" r:id="rId80" name="Control 8">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2056" r:id="rId80" name="Control 8"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2055" r:id="rId81" name="Control 7">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2055" r:id="rId81" name="Control 7"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2054" r:id="rId82" name="Control 6">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2054" r:id="rId82" name="Control 6"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2053" r:id="rId83" name="Control 5">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2053" r:id="rId83" name="Control 5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2052" r:id="rId84" name="Control 4">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2052" r:id="rId84" name="Control 4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2051" r:id="rId85" name="Control 3">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2051" r:id="rId85" name="Control 3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2050" r:id="rId86" name="Control 2">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2050" r:id="rId86" name="Control 2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="2049" r:id="rId87" name="Control 1">
-          <controlPr defaultSize="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="2049" r:id="rId87" name="Control 1"/>
+        <control shapeId="2132" r:id="rId87" name="Control 84"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>

<commit_message>
Delete unused page in BOM excel document
</commit_message>
<xml_diff>
--- a/AxxSolder_hardware/bom/BOM_AxxSolder_V3_0.xlsx
+++ b/AxxSolder_hardware/bom/BOM_AxxSolder_V3_0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\axelj\ownCloud\2_Project\00_AxxProjects\AxxSolder\AxxSolder_hardware\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B6E9833-2ABD-4C0E-8660-C0AB2CDCB7C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B99676-DBAD-421F-B275-721513663C72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{60354D9D-8798-4211-B1E3-D5485177CC9B}"/>
   </bookViews>
@@ -1297,8 +1297,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:M79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K35" sqref="K35"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="K67" sqref="K67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update BOM to correctly color code station and portable parts
</commit_message>
<xml_diff>
--- a/AxxSolder_hardware/bom/BOM_AxxSolder_V3_0.xlsx
+++ b/AxxSolder_hardware/bom/BOM_AxxSolder_V3_0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\axelj\ownCloud\2_Project\00_AxxProjects\AxxSolder\AxxSolder_hardware\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{715871C6-324F-425C-BDB5-024C50E7B537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B818511A-DC5B-4E45-8892-0F442BF0597F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{60354D9D-8798-4211-B1E3-D5485177CC9B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{60354D9D-8798-4211-B1E3-D5485177CC9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -432,9 +432,6 @@
     <t>710-61300611821</t>
   </si>
   <si>
-    <t>Parts for AxxSolder Station only</t>
-  </si>
-  <si>
     <t>Manufacturer</t>
   </si>
   <si>
@@ -456,9 +453,6 @@
     <t>200-TSW10207TS</t>
   </si>
   <si>
-    <t>Parts for AxxSolder Portable only</t>
-  </si>
-  <si>
     <t>80-C0603C102K3G</t>
   </si>
   <si>
@@ -496,9 +490,6 @@
   </si>
   <si>
     <t>Aluminium plate 15x10x3 mm</t>
-  </si>
-  <si>
-    <t>SUM Hardware</t>
   </si>
   <si>
     <t>JBC stand</t>
@@ -767,6 +758,15 @@
   </si>
   <si>
     <t>https://www.aliexpress.com/item/1005005879501637.html?spm=a2g0o.productlist.main.29.2f0682d4ltssPP&amp;algo_pvid=689e6dfe-d7d2-4536-841a-7febab5cb1eb&amp;algo_exp_id=689e6dfe-d7d2-4536-841a-7febab5cb1eb-14&amp;pdp_npi=4%40dis%21SEK%21355.36%21284.29%21%21%21241.05%21192.84%21%40211b600c17175313850401216e65f8%2112000034680227076%21sea%21SE%21134446295%21&amp;curPageLogUid=uptP5hZSIi1p&amp;utparam-url=scene%3Asearch%7Cquery_from%3A</t>
+  </si>
+  <si>
+    <t>Parts for AxxSolder Station</t>
+  </si>
+  <si>
+    <t>Parts for AxxSolder Portable</t>
+  </si>
+  <si>
+    <t>SUM Hardware (portable)</t>
   </si>
 </sst>
 </file>
@@ -1298,8 +1298,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:M79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A56" sqref="A55:A56"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1318,13 +1318,13 @@
   <sheetData>
     <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="18" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>135</v>
+        <v>245</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="22"/>
@@ -1338,7 +1338,7 @@
       <c r="A2" s="19"/>
       <c r="B2" s="21"/>
       <c r="C2" s="4" t="s">
-        <v>143</v>
+        <v>244</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
@@ -1359,30 +1359,30 @@
         <v>2</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="F3" s="16" t="s">
         <v>3</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H3" s="16" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="I3" s="16" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="J3" s="16" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
@@ -1416,7 +1416,7 @@
     </row>
     <row r="5" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>9</v>
@@ -1440,7 +1440,7 @@
         <v>0.17699999999999999</v>
       </c>
       <c r="I5" s="13">
-        <f t="shared" ref="I5:J45" si="0">G5*H5</f>
+        <f t="shared" ref="I5:I45" si="0">G5*H5</f>
         <v>2.8319999999999999</v>
       </c>
       <c r="J5" s="13">
@@ -1450,7 +1450,7 @@
     </row>
     <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>13</v>
@@ -1465,7 +1465,7 @@
         <v>14</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G6" s="1">
         <v>2</v>
@@ -1484,22 +1484,22 @@
     </row>
     <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G7" s="11">
         <v>1</v>
@@ -1518,7 +1518,7 @@
     </row>
     <row r="8" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>15</v>
@@ -1552,7 +1552,7 @@
     </row>
     <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>20</v>
@@ -1586,7 +1586,7 @@
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>23</v>
@@ -1620,7 +1620,7 @@
     </row>
     <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>29</v>
@@ -1654,7 +1654,7 @@
     </row>
     <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>26</v>
@@ -1688,7 +1688,7 @@
     </row>
     <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B13" s="11">
         <v>100</v>
@@ -1722,7 +1722,7 @@
     </row>
     <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>34</v>
@@ -1756,22 +1756,22 @@
     </row>
     <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>39</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D15" s="11" t="s">
         <v>17</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G15" s="11">
         <v>1</v>
@@ -1790,22 +1790,22 @@
     </row>
     <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="G16" s="1">
         <v>1</v>
@@ -1827,7 +1827,7 @@
         <v>41</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C17" s="11" t="s">
         <v>42</v>
@@ -1836,10 +1836,10 @@
         <v>40</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="G17" s="11">
         <v>1</v>
@@ -1964,7 +1964,7 @@
     </row>
     <row r="21" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B21" s="11" t="s">
         <v>58</v>
@@ -2032,22 +2032,22 @@
     </row>
     <row r="23" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D23" s="11" t="s">
         <v>114</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="F23" s="11" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="G23" s="11">
         <v>1</v>
@@ -2103,7 +2103,7 @@
         <v>72</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C25" s="11" t="s">
         <v>73</v>
@@ -2112,10 +2112,10 @@
         <v>56</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="F25" s="11" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="G25" s="11">
         <v>1</v>
@@ -2171,19 +2171,19 @@
         <v>78</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D27" s="11" t="s">
         <v>79</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="F27" s="11" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="G27" s="11">
         <v>3</v>
@@ -2239,19 +2239,19 @@
         <v>84</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D29" s="11" t="s">
         <v>87</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="F29" s="11" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="G29" s="11">
         <v>1</v>
@@ -2307,19 +2307,19 @@
         <v>90</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D31" s="11" t="s">
         <v>87</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="F31" s="11" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G31" s="11">
         <v>1</v>
@@ -2375,19 +2375,19 @@
         <v>96</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D33" s="11" t="s">
         <v>87</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="G33" s="11">
         <v>1</v>
@@ -2474,7 +2474,7 @@
     </row>
     <row r="36" spans="1:10" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>97</v>
@@ -2508,22 +2508,22 @@
     </row>
     <row r="37" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="11" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D37" s="11" t="s">
         <v>87</v>
       </c>
       <c r="E37" s="11" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="F37" s="11" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="G37" s="11">
         <v>1</v>
@@ -2678,22 +2678,22 @@
     </row>
     <row r="42" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>80</v>
       </c>
       <c r="D42" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F42" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>142</v>
       </c>
       <c r="G42" s="1">
         <v>2</v>
@@ -2721,7 +2721,7 @@
         <v>128</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E43" s="11" t="s">
         <v>127</v>
@@ -2780,7 +2780,7 @@
     </row>
     <row r="45" spans="1:10" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="11" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B45" s="11">
         <v>61300611821</v>
@@ -2814,7 +2814,7 @@
     </row>
     <row r="46" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A46" s="7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
@@ -2838,17 +2838,17 @@
     </row>
     <row r="48" spans="1:10" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
       <c r="H48" s="16" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="23" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B49" s="23"/>
       <c r="C49" s="23"/>
@@ -2869,7 +2869,7 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B50" s="10"/>
       <c r="E50">
@@ -2883,13 +2883,13 @@
         <v>5.1100000000000003</v>
       </c>
       <c r="H50" s="9">
-        <f t="shared" ref="H50:H65" si="2">G50*1.25</f>
+        <f t="shared" ref="H50:H64" si="2">G50*1.25</f>
         <v>6.3875000000000002</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B51" s="3"/>
       <c r="E51">
@@ -2909,10 +2909,10 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B52" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E52">
         <v>2</v>
@@ -2931,10 +2931,10 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B53" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="E53">
         <v>2</v>
@@ -2953,10 +2953,10 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B54" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E54">
         <v>2</v>
@@ -2975,10 +2975,10 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B55" s="15" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E55">
         <v>1</v>
@@ -2997,10 +2997,10 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B56" s="15" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E56">
         <v>2</v>
@@ -3019,10 +3019,10 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B57" s="15" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E57">
         <v>1</v>
@@ -3041,7 +3041,7 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E58">
         <v>1</v>
@@ -3060,10 +3060,10 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B59" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="E59">
         <v>4</v>
@@ -3082,10 +3082,10 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B60" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="E60">
         <v>1</v>
@@ -3104,10 +3104,10 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B61" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E61">
         <v>1</v>
@@ -3126,10 +3126,10 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B62" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E62">
         <v>4</v>
@@ -3148,10 +3148,10 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B63" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E63">
         <v>2</v>
@@ -3170,10 +3170,10 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B64" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="E64">
         <v>1</v>
@@ -3192,7 +3192,7 @@
     </row>
     <row r="65" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A65" s="7" t="s">
-        <v>157</v>
+        <v>246</v>
       </c>
       <c r="B65" s="7"/>
       <c r="C65" s="7"/>
@@ -3200,11 +3200,14 @@
       <c r="E65" s="7"/>
       <c r="F65" s="7"/>
       <c r="G65" s="8"/>
-      <c r="H65" s="8"/>
+      <c r="H65" s="8">
+        <f>SUM(H62:H64)+SUM(H58:H60)+SUM(H51:H56)+H49</f>
+        <v>43.418750000000003</v>
+      </c>
     </row>
     <row r="67" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="24" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B67" s="24"/>
       <c r="C67" s="24"/>
@@ -3212,13 +3215,13 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B68" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C68" s="15" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="E68">
         <v>1</v>
@@ -3227,7 +3230,7 @@
         <v>171.4</v>
       </c>
       <c r="G68" s="9">
-        <f t="shared" ref="G68:G70" si="6">F68*E68</f>
+        <f t="shared" ref="G68" si="6">F68*E68</f>
         <v>171.4</v>
       </c>
       <c r="H68">
@@ -3241,7 +3244,7 @@
     </row>
     <row r="70" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="24" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B70" s="24"/>
       <c r="C70" s="24"/>
@@ -3250,10 +3253,10 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>161</v>
-      </c>
-      <c r="B71" t="s">
-        <v>238</v>
+        <v>158</v>
+      </c>
+      <c r="B71" s="15" t="s">
+        <v>235</v>
       </c>
       <c r="E71">
         <v>1</v>
@@ -3277,7 +3280,7 @@
     </row>
     <row r="73" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="24" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B73" s="24"/>
       <c r="G73" s="9"/>
@@ -3285,10 +3288,10 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B74" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="E74">
         <v>1</v>
@@ -3297,20 +3300,20 @@
         <v>66.34</v>
       </c>
       <c r="G74" s="9">
-        <f t="shared" ref="G72:G75" si="7">F74*E74</f>
+        <f t="shared" ref="G74:G75" si="7">F74*E74</f>
         <v>66.34</v>
       </c>
       <c r="H74" s="9">
-        <f t="shared" ref="H72:H79" si="8">G74*1.25</f>
+        <f t="shared" ref="H74:H79" si="8">G74*1.25</f>
         <v>82.925000000000011</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B75" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="E75">
         <v>1</v>
@@ -3335,17 +3338,17 @@
     </row>
     <row r="77" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="24" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B77" s="24"/>
       <c r="H77" s="9"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B78" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E78">
         <v>1</v>
@@ -3364,10 +3367,10 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B79" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="E79">
         <v>1</v>
@@ -3386,6 +3389,7 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A77:B77"/>
     <mergeCell ref="F76:G76"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
@@ -3396,7 +3400,6 @@
     <mergeCell ref="A73:B73"/>
     <mergeCell ref="C67:D67"/>
     <mergeCell ref="C70:D70"/>
-    <mergeCell ref="A77:B77"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D23" r:id="rId1" display="https://eu.mouser.com/manufacturer/cui-devices/" xr:uid="{20A6F0EA-5529-4B15-9D5D-90A5BC0CFECC}"/>
@@ -3404,6 +3407,7 @@
     <hyperlink ref="B56" r:id="rId3" xr:uid="{537D6D9C-9F20-4B7C-8ECD-54BA77D8ACC7}"/>
     <hyperlink ref="B57" r:id="rId4" xr:uid="{DC7B44C9-7248-43F5-9F3E-3B4750BAB0D5}"/>
     <hyperlink ref="C68" r:id="rId5" xr:uid="{1D7E88CD-AFAA-4B97-9D92-1ED605380133}"/>
+    <hyperlink ref="B71" r:id="rId6" xr:uid="{51F49AE6-72ED-40A6-BE54-4BFB91B32B23}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update hardware files to match correctly with current version
</commit_message>
<xml_diff>
--- a/AxxSolder_hardware/bom/BOM_AxxSolder_V3_0.xlsx
+++ b/AxxSolder_hardware/bom/BOM_AxxSolder_V3_0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\axelj\ownCloud\2_Project\00_AxxProjects\AxxSolder\AxxSolder_hardware\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B818511A-DC5B-4E45-8892-0F442BF0597F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B99676-DBAD-421F-B275-721513663C72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{60354D9D-8798-4211-B1E3-D5485177CC9B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{60354D9D-8798-4211-B1E3-D5485177CC9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="238">
   <si>
     <t>References</t>
   </si>
@@ -36,6 +36,9 @@
     <t>Footprint</t>
   </si>
   <si>
+    <t>Manufacturer_Part_Number</t>
+  </si>
+  <si>
     <t>Mouser Part Number</t>
   </si>
   <si>
@@ -432,6 +435,9 @@
     <t>710-61300611821</t>
   </si>
   <si>
+    <t>Parts for AxxSolder Station only</t>
+  </si>
+  <si>
     <t>Manufacturer</t>
   </si>
   <si>
@@ -453,6 +459,9 @@
     <t>200-TSW10207TS</t>
   </si>
   <si>
+    <t>Parts for AxxSolder Portable only</t>
+  </si>
+  <si>
     <t>80-C0603C102K3G</t>
   </si>
   <si>
@@ -492,6 +501,9 @@
     <t>Aluminium plate 15x10x3 mm</t>
   </si>
   <si>
+    <t>SUM Hardware</t>
+  </si>
+  <si>
     <t>JBC stand</t>
   </si>
   <si>
@@ -510,6 +522,18 @@
     <t>T210 handle piece</t>
   </si>
   <si>
+    <t>c210-0008 tip</t>
+  </si>
+  <si>
+    <t>SUM JBC stand and handle</t>
+  </si>
+  <si>
+    <t>TOTAL Sum with genuine JBC handle and stand</t>
+  </si>
+  <si>
+    <t>TOTAL Sum with non-genuine JBC stand</t>
+  </si>
+  <si>
     <t>C3, C9, C14, C15, C16, C17, C18, C21, C22, C23, C24, C25, C26, C27, C28, C29, C33</t>
   </si>
   <si>
@@ -639,6 +663,10 @@
     <t>179-RIC1131S15D7GSMT</t>
   </si>
   <si>
+    <t xml:space="preserve">PCB - Development was done with PCBs from PCBWay, 2 layer, Immersion gold(ENIG) (1U"), + stencil
+</t>
+  </si>
+  <si>
     <t>https://eu.mouser.com/ProductDetail/Davies-Molding/1101?qs=byeeYqUIh0PVJzrDf6EcyQ%3D%3D</t>
   </si>
   <si>
@@ -712,61 +740,6 @@
   </si>
   <si>
     <t>595-INA281A5QDBVRQ1</t>
-  </si>
-  <si>
-    <t>Price total inc tax</t>
-  </si>
-  <si>
-    <t>MPN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PCB  (Development was done with PCBs from PCBWay, 2 layer, Immersion gold(ENIG) (1U")) + stencil
-</t>
-  </si>
-  <si>
-    <t>Price inc tax</t>
-  </si>
-  <si>
-    <t>For the aluminium rest (not mandatory)</t>
-  </si>
-  <si>
-    <t>https://eleshop.eu/jbc-ad-sf-stand-for-t245-and-t210.html</t>
-  </si>
-  <si>
-    <t>https://www.aliexpress.com/i/1005005756505193.html</t>
-  </si>
-  <si>
-    <t>https://www.jbctools.com/t210-a-precision-handle-product-48.html</t>
-  </si>
-  <si>
-    <t>c210-008 tip</t>
-  </si>
-  <si>
-    <t>https://www.jbctools.com/c210008-chisel-cartridge-13-x-06-product-183.html</t>
-  </si>
-  <si>
-    <t>Non-genuine JBC T210 handle piece</t>
-  </si>
-  <si>
-    <t>Aixun T210 handle piece</t>
-  </si>
-  <si>
-    <t>Aixun c210-008 tip</t>
-  </si>
-  <si>
-    <t>https://www.aliexpress.com/item/1005005081918036.html?algo_pvid=78d4a98a-6d47-43e1-8e91-4c3c1ae5cf4d&amp;aem_p4p_detail=20240604130221402631312959600000935203&amp;algo_exp_id=78d4a98a-6d47-43e1-8e91-4c3c1ae5cf4d-2&amp;pdp_npi=4%40dis%21SEK%21459.81%21229.91%21%21%2143.04%2121.52%21%40211b600d17175313411604987e9089%2112000031572016441%21sea%21SE%21134446295%21&amp;curPageLogUid=ntxK57ZqBX5y&amp;utparam-url=scene%3Asearch%7Cquery_from%3A&amp;search_p4p_id=20240604130221402631312959600000935203_3</t>
-  </si>
-  <si>
-    <t>https://www.aliexpress.com/item/1005005879501637.html?spm=a2g0o.productlist.main.29.2f0682d4ltssPP&amp;algo_pvid=689e6dfe-d7d2-4536-841a-7febab5cb1eb&amp;algo_exp_id=689e6dfe-d7d2-4536-841a-7febab5cb1eb-14&amp;pdp_npi=4%40dis%21SEK%21355.36%21284.29%21%21%21241.05%21192.84%21%40211b600c17175313850401216e65f8%2112000034680227076%21sea%21SE%21134446295%21&amp;curPageLogUid=uptP5hZSIi1p&amp;utparam-url=scene%3Asearch%7Cquery_from%3A</t>
-  </si>
-  <si>
-    <t>Parts for AxxSolder Station</t>
-  </si>
-  <si>
-    <t>Parts for AxxSolder Portable</t>
-  </si>
-  <si>
-    <t>SUM Hardware (portable)</t>
   </si>
 </sst>
 </file>
@@ -779,7 +752,7 @@
     <numFmt numFmtId="166" formatCode="#,##0.00\ [$€-1];[Red]\-#,##0.00\ [$€-1]"/>
     <numFmt numFmtId="167" formatCode="_-* #,##0.00\ [$€-1]_-;\-* #,##0.00\ [$€-1]_-;_-* &quot;-&quot;??\ [$€-1]_-;_-@_-"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -818,6 +791,24 @@
     <font>
       <b/>
       <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <u/>
+      <sz val="28"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <u/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -920,9 +911,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -940,6 +931,7 @@
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -952,11 +944,14 @@
     <xf numFmtId="167" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -974,9 +969,13 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1298,8 +1297,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:M79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C82" sqref="C82"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="K67" sqref="K67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1307,1446 +1306,1280 @@
     <col min="1" max="1" width="50.7109375" customWidth="1"/>
     <col min="2" max="2" width="32.28515625" customWidth="1"/>
     <col min="3" max="3" width="34.85546875" customWidth="1"/>
-    <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="23.140625" customWidth="1"/>
+    <col min="4" max="4" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" customWidth="1"/>
     <col min="8" max="8" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="B1" s="20" t="s">
-        <v>214</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
+    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>223</v>
+      </c>
+      <c r="C1" s="24"/>
+      <c r="D1" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-    </row>
-    <row r="2" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="19"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="D2" s="5"/>
+    </row>
+    <row r="2" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="21"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="4" t="s">
+        <v>144</v>
+      </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-    </row>
-    <row r="3" spans="1:10" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="16" t="s">
+    </row>
+    <row r="3" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="16" t="s">
+      <c r="B3" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>230</v>
-      </c>
-      <c r="F3" s="16" t="s">
+      <c r="D3" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="E3" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="H3" s="16" t="s">
-        <v>200</v>
-      </c>
-      <c r="I3" s="16" t="s">
-        <v>201</v>
-      </c>
-      <c r="J3" s="16" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F3" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="I3" s="17" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G4" s="1">
         <v>17</v>
       </c>
-      <c r="H4" s="13">
+      <c r="H4" s="14">
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="I4" s="13">
+      <c r="I4" s="14">
         <f>G4*H4</f>
         <v>0.73099999999999998</v>
       </c>
-      <c r="J4" s="13">
-        <f>1.25*I4</f>
-        <v>0.91374999999999995</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="11" t="s">
+    </row>
+    <row r="5" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="B5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="C5" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="E5" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="11">
+      <c r="F5" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="12">
         <v>16</v>
       </c>
-      <c r="H5" s="14">
+      <c r="H5" s="15">
         <v>0.17699999999999999</v>
       </c>
-      <c r="I5" s="13">
+      <c r="I5" s="14">
         <f t="shared" ref="I5:I45" si="0">G5*H5</f>
         <v>2.8319999999999999</v>
       </c>
-      <c r="J5" s="13">
-        <f t="shared" ref="J5:J45" si="1">1.25*I5</f>
-        <v>3.54</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="G6" s="1">
         <v>2</v>
       </c>
-      <c r="H6" s="13">
+      <c r="H6" s="14">
         <v>9.2999999999999999E-2</v>
       </c>
-      <c r="I6" s="13">
+      <c r="I6" s="14">
         <f t="shared" si="0"/>
         <v>0.186</v>
       </c>
-      <c r="J6" s="13">
-        <f t="shared" si="1"/>
-        <v>0.23249999999999998</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>191</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>192</v>
-      </c>
-      <c r="G7" s="11">
-        <v>1</v>
-      </c>
-      <c r="H7" s="14">
+    </row>
+    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="G7" s="12">
+        <v>1</v>
+      </c>
+      <c r="H7" s="15">
         <v>0.61399999999999999</v>
       </c>
-      <c r="I7" s="13">
+      <c r="I7" s="14">
         <f t="shared" si="0"/>
         <v>0.61399999999999999</v>
       </c>
-      <c r="J7" s="13">
-        <f t="shared" si="1"/>
-        <v>0.76749999999999996</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G8" s="1">
         <v>20</v>
       </c>
-      <c r="H8" s="13">
+      <c r="H8" s="14">
         <v>0.125</v>
       </c>
-      <c r="I8" s="13">
+      <c r="I8" s="14">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="J8" s="13">
-        <f t="shared" si="1"/>
-        <v>3.125</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="11" t="s">
+    </row>
+    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="11" t="s">
+      <c r="D9" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="11">
+      <c r="F9" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" s="12">
         <v>5</v>
       </c>
-      <c r="H9" s="14">
+      <c r="H9" s="15">
         <v>0.14000000000000001</v>
       </c>
-      <c r="I9" s="13">
+      <c r="I9" s="14">
         <f t="shared" si="0"/>
         <v>0.70000000000000007</v>
       </c>
-      <c r="J9" s="13">
-        <f t="shared" si="1"/>
-        <v>0.87500000000000011</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G10" s="1">
         <v>4</v>
       </c>
-      <c r="H10" s="13">
+      <c r="H10" s="14">
         <v>0.214</v>
       </c>
-      <c r="I10" s="13">
+      <c r="I10" s="14">
         <f t="shared" si="0"/>
         <v>0.85599999999999998</v>
       </c>
-      <c r="J10" s="13">
-        <f t="shared" si="1"/>
-        <v>1.07</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="11" t="s">
-        <v>170</v>
-      </c>
-      <c r="B11" s="11" t="s">
+    </row>
+    <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" s="12">
+        <v>4</v>
+      </c>
+      <c r="H11" s="15">
+        <v>0.121</v>
+      </c>
+      <c r="I11" s="14">
+        <f t="shared" si="0"/>
+        <v>0.48399999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="G11" s="11">
-        <v>4</v>
-      </c>
-      <c r="H11" s="14">
-        <v>0.121</v>
-      </c>
-      <c r="I11" s="13">
-        <f t="shared" si="0"/>
-        <v>0.48399999999999999</v>
-      </c>
-      <c r="J11" s="13">
-        <f t="shared" si="1"/>
-        <v>0.60499999999999998</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="G12" s="1">
         <v>2</v>
       </c>
-      <c r="H12" s="13">
+      <c r="H12" s="14">
         <v>0.121</v>
       </c>
-      <c r="I12" s="13">
+      <c r="I12" s="14">
         <f t="shared" si="0"/>
         <v>0.24199999999999999</v>
       </c>
-      <c r="J12" s="13">
-        <f t="shared" si="1"/>
-        <v>0.30249999999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="11" t="s">
-        <v>172</v>
-      </c>
-      <c r="B13" s="11">
+    </row>
+    <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="B13" s="12">
         <v>100</v>
       </c>
-      <c r="C13" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="11" t="s">
+      <c r="C13" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F13" s="11" t="s">
+      <c r="D13" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="G13" s="11">
+      <c r="F13" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13" s="12">
         <v>2</v>
       </c>
-      <c r="H13" s="14">
+      <c r="H13" s="15">
         <v>0.307</v>
       </c>
-      <c r="I13" s="13">
+      <c r="I13" s="14">
         <f t="shared" si="0"/>
         <v>0.61399999999999999</v>
       </c>
-      <c r="J13" s="13">
-        <f t="shared" si="1"/>
-        <v>0.76749999999999996</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G14" s="1">
         <v>1</v>
       </c>
-      <c r="H14" s="13">
+      <c r="H14" s="14">
         <v>0.753</v>
       </c>
-      <c r="I14" s="13">
+      <c r="I14" s="14">
         <f t="shared" si="0"/>
         <v>0.753</v>
       </c>
-      <c r="J14" s="13">
-        <f t="shared" si="1"/>
-        <v>0.94125000000000003</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>193</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="G15" s="11">
-        <v>1</v>
-      </c>
-      <c r="H15" s="14">
+    </row>
+    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>201</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="G15" s="12">
+        <v>1</v>
+      </c>
+      <c r="H15" s="15">
         <v>9.2999999999999999E-2</v>
       </c>
-      <c r="I15" s="13">
+      <c r="I15" s="14">
         <f t="shared" si="0"/>
         <v>9.2999999999999999E-2</v>
       </c>
-      <c r="J15" s="13">
-        <f t="shared" si="1"/>
-        <v>0.11624999999999999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>224</v>
+        <v>233</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>225</v>
+        <v>234</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>226</v>
+        <v>235</v>
       </c>
       <c r="G16" s="1">
         <v>1</v>
       </c>
-      <c r="H16" s="13">
+      <c r="H16" s="14">
         <v>0.40899999999999997</v>
       </c>
-      <c r="I16" s="13">
+      <c r="I16" s="14">
         <f t="shared" si="0"/>
         <v>0.40899999999999997</v>
       </c>
-      <c r="J16" s="13">
-        <f t="shared" si="1"/>
-        <v>0.51124999999999998</v>
-      </c>
     </row>
     <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B17" s="11" t="s">
-        <v>177</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>177</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>195</v>
-      </c>
-      <c r="G17" s="11">
-        <v>1</v>
-      </c>
-      <c r="H17" s="14">
+      <c r="E17" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="G17" s="12">
+        <v>1</v>
+      </c>
+      <c r="H17" s="15">
         <v>0.753</v>
       </c>
-      <c r="I17" s="13">
+      <c r="I17" s="14">
         <f t="shared" si="0"/>
         <v>0.753</v>
-      </c>
-      <c r="J17" s="13">
-        <f t="shared" si="1"/>
-        <v>0.94125000000000003</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="F18" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G18" s="1">
         <v>4</v>
       </c>
-      <c r="H18" s="13">
+      <c r="H18" s="14">
         <v>0.112</v>
       </c>
-      <c r="I18" s="13">
+      <c r="I18" s="14">
         <f t="shared" si="0"/>
         <v>0.44800000000000001</v>
       </c>
-      <c r="J18" s="13">
-        <f t="shared" si="1"/>
-        <v>0.56000000000000005</v>
-      </c>
     </row>
     <row r="19" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="B19" s="11" t="s">
+      <c r="A19" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="B19" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="C19" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="E19" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="F19" s="11" t="s">
+      <c r="D19" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="G19" s="11">
+      <c r="E19" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="G19" s="12">
         <v>2</v>
       </c>
-      <c r="H19" s="14">
+      <c r="H19" s="15">
         <v>0.19500000000000001</v>
       </c>
-      <c r="I19" s="13">
+      <c r="I19" s="14">
         <f t="shared" si="0"/>
         <v>0.39</v>
       </c>
-      <c r="J19" s="13">
-        <f t="shared" si="1"/>
-        <v>0.48750000000000004</v>
-      </c>
-      <c r="K19" s="12"/>
+      <c r="K19" s="13"/>
       <c r="M19" s="6"/>
     </row>
     <row r="20" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="F20" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G20" s="1">
         <v>2</v>
       </c>
-      <c r="H20" s="13">
+      <c r="H20" s="14">
         <v>0.4</v>
       </c>
-      <c r="I20" s="13">
+      <c r="I20" s="14">
         <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
-      <c r="J20" s="13">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="K20" s="12"/>
+      <c r="K20" s="13"/>
       <c r="M20" s="6"/>
     </row>
     <row r="21" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="11" t="s">
-        <v>178</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="C21" s="11" t="s">
+      <c r="A21" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="B21" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="C21" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="D21" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="F21" s="11" t="s">
+      <c r="E21" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="G21" s="11">
+      <c r="F21" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="G21" s="12">
         <v>2</v>
       </c>
-      <c r="H21" s="14">
+      <c r="H21" s="15">
         <v>0.372</v>
       </c>
-      <c r="I21" s="13">
+      <c r="I21" s="14">
         <f t="shared" si="0"/>
         <v>0.74399999999999999</v>
-      </c>
-      <c r="J21" s="13">
-        <f t="shared" si="1"/>
-        <v>0.92999999999999994</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E22" s="1">
         <v>4311</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G22" s="1">
         <v>1</v>
       </c>
-      <c r="H22" s="13">
+      <c r="H22" s="14">
         <v>18.55</v>
       </c>
-      <c r="I22" s="13">
+      <c r="I22" s="14">
         <f t="shared" si="0"/>
         <v>18.55</v>
       </c>
-      <c r="J22" s="13">
-        <f t="shared" si="1"/>
-        <v>23.1875</v>
-      </c>
     </row>
     <row r="23" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="11" t="s">
-        <v>179</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>202</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>202</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="E23" s="11" t="s">
-        <v>202</v>
-      </c>
-      <c r="F23" s="11" t="s">
-        <v>203</v>
-      </c>
-      <c r="G23" s="11">
-        <v>1</v>
-      </c>
-      <c r="H23" s="14">
+      <c r="A23" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="G23" s="12">
+        <v>1</v>
+      </c>
+      <c r="H23" s="15">
         <v>2.37</v>
       </c>
-      <c r="I23" s="13">
+      <c r="I23" s="14">
         <f t="shared" si="0"/>
         <v>2.37</v>
-      </c>
-      <c r="J23" s="13">
-        <f t="shared" si="1"/>
-        <v>2.9625000000000004</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G24" s="1">
         <v>1</v>
       </c>
-      <c r="H24" s="13">
+      <c r="H24" s="14">
         <v>1.6</v>
       </c>
-      <c r="I24" s="13">
+      <c r="I24" s="14">
         <f t="shared" si="0"/>
         <v>1.6</v>
       </c>
-      <c r="J24" s="13">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
     </row>
     <row r="25" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>223</v>
-      </c>
-      <c r="C25" s="11" t="s">
+      <c r="A25" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="D25" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="E25" s="11" t="s">
-        <v>223</v>
-      </c>
-      <c r="F25" s="11" t="s">
-        <v>222</v>
-      </c>
-      <c r="G25" s="11">
-        <v>1</v>
-      </c>
-      <c r="H25" s="14">
+      <c r="B25" s="12" t="s">
+        <v>232</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>232</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="G25" s="12">
+        <v>1</v>
+      </c>
+      <c r="H25" s="15">
         <v>2.5499999999999998</v>
       </c>
-      <c r="I25" s="13">
+      <c r="I25" s="14">
         <f t="shared" si="0"/>
         <v>2.5499999999999998</v>
-      </c>
-      <c r="J25" s="13">
-        <f t="shared" si="1"/>
-        <v>3.1875</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="F26" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G26" s="1">
         <v>1</v>
       </c>
-      <c r="H26" s="13">
+      <c r="H26" s="14">
         <v>0.72499999999999998</v>
       </c>
-      <c r="I26" s="13">
+      <c r="I26" s="14">
         <f t="shared" si="0"/>
         <v>0.72499999999999998</v>
       </c>
-      <c r="J26" s="13">
-        <f t="shared" si="1"/>
-        <v>0.90625</v>
-      </c>
     </row>
     <row r="27" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="B27" s="11" t="s">
-        <v>180</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>180</v>
-      </c>
-      <c r="D27" s="11" t="s">
+      <c r="A27" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="E27" s="11" t="s">
-        <v>180</v>
-      </c>
-      <c r="F27" s="11" t="s">
-        <v>196</v>
-      </c>
-      <c r="G27" s="11">
+      <c r="B27" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="G27" s="12">
         <v>3</v>
       </c>
-      <c r="H27" s="14">
+      <c r="H27" s="15">
         <v>0.54900000000000004</v>
       </c>
-      <c r="I27" s="13">
+      <c r="I27" s="14">
         <f t="shared" si="0"/>
         <v>1.6470000000000002</v>
-      </c>
-      <c r="J27" s="13">
-        <f t="shared" si="1"/>
-        <v>2.0587500000000003</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G28" s="1">
         <v>1</v>
       </c>
-      <c r="H28" s="13">
+      <c r="H28" s="14">
         <v>0.17699999999999999</v>
       </c>
-      <c r="I28" s="13">
+      <c r="I28" s="14">
         <f t="shared" si="0"/>
         <v>0.17699999999999999</v>
       </c>
-      <c r="J28" s="13">
-        <f t="shared" si="1"/>
-        <v>0.22125</v>
-      </c>
     </row>
     <row r="29" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="B29" s="11" t="s">
-        <v>181</v>
-      </c>
-      <c r="C29" s="11" t="s">
-        <v>182</v>
-      </c>
-      <c r="D29" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="E29" s="11" t="s">
-        <v>181</v>
-      </c>
-      <c r="F29" s="11" t="s">
-        <v>197</v>
-      </c>
-      <c r="G29" s="11">
-        <v>1</v>
-      </c>
-      <c r="H29" s="14">
+      <c r="A29" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="E29" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="G29" s="12">
+        <v>1</v>
+      </c>
+      <c r="H29" s="15">
         <v>0.38100000000000001</v>
       </c>
-      <c r="I29" s="13">
+      <c r="I29" s="14">
         <f t="shared" si="0"/>
         <v>0.38100000000000001</v>
-      </c>
-      <c r="J29" s="13">
-        <f t="shared" si="1"/>
-        <v>0.47625000000000001</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F30" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="F30" s="1" t="s">
+      <c r="G30" s="1">
+        <v>1</v>
+      </c>
+      <c r="H30" s="14">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="I30" s="14">
+        <f t="shared" si="0"/>
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="D31" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="G30" s="1">
-        <v>1</v>
-      </c>
-      <c r="H30" s="13">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="I30" s="13">
-        <f t="shared" si="0"/>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="J30" s="13">
-        <f t="shared" si="1"/>
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="B31" s="11" t="s">
-        <v>183</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>184</v>
-      </c>
-      <c r="D31" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="E31" s="11" t="s">
-        <v>183</v>
-      </c>
-      <c r="F31" s="11" t="s">
-        <v>198</v>
-      </c>
-      <c r="G31" s="11">
-        <v>1</v>
-      </c>
-      <c r="H31" s="14">
+      <c r="E31" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="G31" s="12">
+        <v>1</v>
+      </c>
+      <c r="H31" s="15">
         <v>0.96699999999999997</v>
       </c>
-      <c r="I31" s="13">
+      <c r="I31" s="14">
         <f t="shared" si="0"/>
         <v>0.96699999999999997</v>
-      </c>
-      <c r="J31" s="13">
-        <f t="shared" si="1"/>
-        <v>1.20875</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="G32" s="1">
+        <v>1</v>
+      </c>
+      <c r="H32" s="14">
+        <v>5.65</v>
+      </c>
+      <c r="I32" s="14">
+        <f t="shared" si="0"/>
+        <v>5.65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="D33" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="F33" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="G33" s="12">
+        <v>1</v>
+      </c>
+      <c r="H33" s="15">
+        <v>0.32600000000000001</v>
+      </c>
+      <c r="I33" s="14">
+        <f t="shared" si="0"/>
+        <v>0.32600000000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G34" s="1">
+        <v>1</v>
+      </c>
+      <c r="H34" s="14">
+        <v>2.52</v>
+      </c>
+      <c r="I34" s="14">
+        <f t="shared" si="0"/>
+        <v>2.52</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="G32" s="1">
-        <v>1</v>
-      </c>
-      <c r="H32" s="13">
-        <v>5.65</v>
-      </c>
-      <c r="I32" s="13">
-        <f t="shared" si="0"/>
-        <v>5.65</v>
-      </c>
-      <c r="J32" s="13">
-        <f t="shared" si="1"/>
-        <v>7.0625</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="B33" s="11" t="s">
-        <v>185</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>184</v>
-      </c>
-      <c r="D33" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="E33" s="11" t="s">
-        <v>185</v>
-      </c>
-      <c r="F33" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="G33" s="11">
-        <v>1</v>
-      </c>
-      <c r="H33" s="14">
-        <v>0.32600000000000001</v>
-      </c>
-      <c r="I33" s="13">
-        <f t="shared" si="0"/>
-        <v>0.32600000000000001</v>
-      </c>
-      <c r="J33" s="13">
-        <f t="shared" si="1"/>
-        <v>0.40750000000000003</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
+      <c r="B35" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="D35" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="E35" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="F35" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="G35" s="12">
+        <v>1</v>
+      </c>
+      <c r="H35" s="15">
+        <v>2.64</v>
+      </c>
+      <c r="I35" s="14">
+        <f t="shared" si="0"/>
+        <v>2.64</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F36" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F34" s="1" t="s">
+      <c r="G36" s="1">
+        <v>1</v>
+      </c>
+      <c r="H36" s="14">
+        <v>5.22</v>
+      </c>
+      <c r="I36" s="14">
+        <f t="shared" si="0"/>
+        <v>5.22</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="B37" s="12" t="s">
+        <v>236</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="D37" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="E37" s="12" t="s">
+        <v>236</v>
+      </c>
+      <c r="F37" s="12" t="s">
+        <v>237</v>
+      </c>
+      <c r="G37" s="12">
+        <v>1</v>
+      </c>
+      <c r="H37" s="15">
+        <v>2.74</v>
+      </c>
+      <c r="I37" s="14">
+        <f t="shared" si="0"/>
+        <v>2.74</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G38" s="1">
+        <v>1</v>
+      </c>
+      <c r="H38" s="14">
+        <v>2.71</v>
+      </c>
+      <c r="I38" s="14">
+        <f t="shared" si="0"/>
+        <v>2.71</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="B39" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="D39" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="G34" s="1">
-        <v>1</v>
-      </c>
-      <c r="H34" s="13">
-        <v>2.52</v>
-      </c>
-      <c r="I34" s="13">
-        <f t="shared" si="0"/>
-        <v>2.52</v>
-      </c>
-      <c r="J34" s="13">
-        <f t="shared" si="1"/>
-        <v>3.15</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="B35" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="C35" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="D35" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="E35" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="F35" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="G35" s="11">
-        <v>1</v>
-      </c>
-      <c r="H35" s="14">
-        <v>2.64</v>
-      </c>
-      <c r="I35" s="13">
-        <f t="shared" si="0"/>
-        <v>2.64</v>
-      </c>
-      <c r="J35" s="13">
-        <f t="shared" si="1"/>
-        <v>3.3000000000000003</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="G36" s="1">
-        <v>1</v>
-      </c>
-      <c r="H36" s="13">
-        <v>5.22</v>
-      </c>
-      <c r="I36" s="13">
-        <f t="shared" si="0"/>
-        <v>5.22</v>
-      </c>
-      <c r="J36" s="13">
-        <f t="shared" si="1"/>
-        <v>6.5249999999999995</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="11" t="s">
-        <v>187</v>
-      </c>
-      <c r="B37" s="11" t="s">
-        <v>227</v>
-      </c>
-      <c r="C37" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="D37" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="E37" s="11" t="s">
-        <v>227</v>
-      </c>
-      <c r="F37" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="G37" s="11">
-        <v>1</v>
-      </c>
-      <c r="H37" s="14">
-        <v>2.74</v>
-      </c>
-      <c r="I37" s="13">
-        <f t="shared" si="0"/>
-        <v>2.74</v>
-      </c>
-      <c r="J37" s="13">
-        <f t="shared" si="1"/>
-        <v>3.4250000000000003</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="G38" s="1">
-        <v>1</v>
-      </c>
-      <c r="H38" s="13">
-        <v>2.71</v>
-      </c>
-      <c r="I38" s="13">
-        <f t="shared" si="0"/>
-        <v>2.71</v>
-      </c>
-      <c r="J38" s="13">
-        <f t="shared" si="1"/>
-        <v>3.3875000000000002</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="B39" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="C39" s="11" t="s">
+      <c r="E39" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="D39" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="E39" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="F39" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="G39" s="11">
-        <v>1</v>
-      </c>
-      <c r="H39" s="14">
+      <c r="F39" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="G39" s="12">
+        <v>1</v>
+      </c>
+      <c r="H39" s="15">
         <v>0.995</v>
       </c>
-      <c r="I39" s="13">
+      <c r="I39" s="14">
         <f t="shared" si="0"/>
         <v>0.995</v>
       </c>
-      <c r="J39" s="13">
-        <f t="shared" si="1"/>
-        <v>1.2437499999999999</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="40" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B40" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G40" s="1">
+        <v>1</v>
+      </c>
+      <c r="H40" s="14">
+        <v>0.96699999999999997</v>
+      </c>
+      <c r="I40" s="14">
+        <f t="shared" si="0"/>
+        <v>0.96699999999999997</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="C40" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="G40" s="1">
-        <v>1</v>
-      </c>
-      <c r="H40" s="13">
-        <v>0.96699999999999997</v>
-      </c>
-      <c r="I40" s="13">
-        <f t="shared" si="0"/>
-        <v>0.96699999999999997</v>
-      </c>
-      <c r="J40" s="13">
-        <f t="shared" si="1"/>
-        <v>1.20875</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="11" t="s">
+      <c r="B41" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="C41" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D41" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="E41" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="F41" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="B41" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="C41" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="D41" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="E41" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="F41" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="G41" s="11">
-        <v>1</v>
-      </c>
-      <c r="H41" s="14">
+      <c r="G41" s="12">
+        <v>1</v>
+      </c>
+      <c r="H41" s="15">
         <v>0.13</v>
       </c>
-      <c r="I41" s="13">
+      <c r="I41" s="14">
         <f t="shared" si="0"/>
         <v>0.13</v>
       </c>
-      <c r="J41" s="13">
-        <f t="shared" si="1"/>
-        <v>0.16250000000000001</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="42" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="G42" s="1">
         <v>2</v>
       </c>
-      <c r="H42" s="13">
+      <c r="H42" s="14">
         <v>9.2999999999999999E-2</v>
       </c>
-      <c r="I42" s="13">
+      <c r="I42" s="14">
         <f t="shared" si="0"/>
         <v>0.186</v>
       </c>
-      <c r="J42" s="13">
-        <f t="shared" si="1"/>
-        <v>0.23249999999999998</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="B43" s="11" t="s">
+    </row>
+    <row r="43" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="C43" s="11" t="s">
+      <c r="B43" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="D43" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="E43" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="F43" s="11" t="s">
+      <c r="C43" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="G43" s="11">
-        <v>1</v>
-      </c>
-      <c r="H43" s="14">
+      <c r="D43" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="E43" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="F43" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="G43" s="12">
+        <v>1</v>
+      </c>
+      <c r="H43" s="15">
         <v>1.26</v>
       </c>
-      <c r="I43" s="13">
+      <c r="I43" s="14">
         <f t="shared" si="0"/>
         <v>1.26</v>
       </c>
-      <c r="J43" s="13">
-        <f t="shared" si="1"/>
-        <v>1.575</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="44" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B44" s="1">
         <v>691243110009</v>
@@ -2755,79 +2588,70 @@
         <v>691243110009</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E44" s="1">
         <v>691243110009</v>
       </c>
       <c r="F44" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G44" s="1">
+        <v>1</v>
+      </c>
+      <c r="H44" s="14">
+        <v>3.7</v>
+      </c>
+      <c r="I44" s="14">
+        <f t="shared" si="0"/>
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="B45" s="12">
+        <v>61300611821</v>
+      </c>
+      <c r="C45" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="D45" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="G44" s="1">
-        <v>1</v>
-      </c>
-      <c r="H44" s="13">
-        <v>3.7</v>
-      </c>
-      <c r="I44" s="13">
-        <f t="shared" si="0"/>
-        <v>3.7</v>
-      </c>
-      <c r="J44" s="13">
-        <f t="shared" si="1"/>
-        <v>4.625</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="11" t="s">
-        <v>190</v>
-      </c>
-      <c r="B45" s="11">
+      <c r="E45" s="12">
         <v>61300611821</v>
       </c>
-      <c r="C45" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="D45" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="E45" s="11">
-        <v>61300611821</v>
-      </c>
-      <c r="F45" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="G45" s="11">
-        <v>1</v>
-      </c>
-      <c r="H45" s="14">
+      <c r="F45" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="G45" s="12">
+        <v>1</v>
+      </c>
+      <c r="H45" s="15">
         <v>0.33500000000000002</v>
       </c>
-      <c r="I45" s="13">
+      <c r="I45" s="14">
         <f t="shared" si="0"/>
         <v>0.33500000000000002</v>
       </c>
-      <c r="J45" s="13">
-        <f t="shared" si="1"/>
-        <v>0.41875000000000001</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="46" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A46" s="7" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
       <c r="D46" s="7"/>
       <c r="E46" s="7"/>
       <c r="F46" s="7"/>
-      <c r="I46" s="8"/>
-      <c r="J46" s="8">
-        <f>SUM(J4:J45)</f>
-        <v>96.11875000000002</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="I46" s="8">
+        <f>SUM(I4:I45)</f>
+        <v>76.894999999999996</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A47" s="7"/>
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
@@ -2836,22 +2660,19 @@
       <c r="F47" s="7"/>
       <c r="G47" s="8"/>
     </row>
-    <row r="48" spans="1:10" ht="36" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:9" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="5" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
-      <c r="H48" s="16" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="23" t="s">
-        <v>231</v>
-      </c>
-      <c r="B49" s="23"/>
-      <c r="C49" s="23"/>
+    </row>
+    <row r="49" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="26" t="s">
+        <v>212</v>
+      </c>
+      <c r="B49" s="26"/>
+      <c r="C49" s="26"/>
       <c r="E49">
         <v>1</v>
       </c>
@@ -2862,14 +2683,10 @@
         <f>F49*E49</f>
         <v>12.62</v>
       </c>
-      <c r="H49" s="9">
-        <f>G49*1.25</f>
-        <v>15.774999999999999</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="10" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B50" s="10"/>
       <c r="E50">
@@ -2882,14 +2699,10 @@
         <f>F50*E50</f>
         <v>5.1100000000000003</v>
       </c>
-      <c r="H50" s="9">
-        <f t="shared" ref="H50:H64" si="2">G50*1.25</f>
-        <v>6.3875000000000002</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B51" s="3"/>
       <c r="E51">
@@ -2902,17 +2715,13 @@
         <f>F51*E51</f>
         <v>6.11</v>
       </c>
-      <c r="H51" s="9">
-        <f t="shared" si="2"/>
-        <v>7.6375000000000002</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
       <c r="B52" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="E52">
         <v>2</v>
@@ -2921,20 +2730,16 @@
         <v>0.94899999999999995</v>
       </c>
       <c r="G52" s="9">
-        <f t="shared" ref="G52:G64" si="3">F52*E52</f>
+        <f t="shared" ref="G52:G64" si="1">F52*E52</f>
         <v>1.8979999999999999</v>
       </c>
-      <c r="H52" s="9">
-        <f t="shared" si="2"/>
-        <v>2.3725000000000001</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
       <c r="B53" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="E53">
         <v>2</v>
@@ -2943,20 +2748,16 @@
         <v>1.37</v>
       </c>
       <c r="G53" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>2.74</v>
       </c>
-      <c r="H53" s="9">
-        <f t="shared" si="2"/>
-        <v>3.4250000000000003</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>220</v>
+        <v>229</v>
       </c>
       <c r="B54" t="s">
-        <v>215</v>
+        <v>224</v>
       </c>
       <c r="E54">
         <v>2</v>
@@ -2965,20 +2766,16 @@
         <v>0.84</v>
       </c>
       <c r="G54" s="9">
-        <f t="shared" ref="G54" si="4">F54*E54</f>
+        <f t="shared" ref="G54" si="2">F54*E54</f>
         <v>1.68</v>
       </c>
-      <c r="H54" s="9">
-        <f t="shared" si="2"/>
-        <v>2.1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>147</v>
-      </c>
-      <c r="B55" s="15" t="s">
-        <v>204</v>
+        <v>150</v>
+      </c>
+      <c r="B55" s="16" t="s">
+        <v>213</v>
       </c>
       <c r="E55">
         <v>1</v>
@@ -2987,20 +2784,16 @@
         <v>0.875</v>
       </c>
       <c r="G55" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.875</v>
       </c>
-      <c r="H55" s="9">
-        <f t="shared" si="2"/>
-        <v>1.09375</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>205</v>
-      </c>
-      <c r="B56" s="15" t="s">
-        <v>206</v>
+        <v>214</v>
+      </c>
+      <c r="B56" s="16" t="s">
+        <v>215</v>
       </c>
       <c r="E56">
         <v>2</v>
@@ -3009,20 +2802,16 @@
         <v>0.85599999999999998</v>
       </c>
       <c r="G56" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>1.712</v>
       </c>
-      <c r="H56" s="9">
-        <f t="shared" si="2"/>
-        <v>2.14</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
-        <v>208</v>
-      </c>
-      <c r="B57" s="15" t="s">
-        <v>221</v>
+        <v>217</v>
+      </c>
+      <c r="B57" s="16" t="s">
+        <v>230</v>
       </c>
       <c r="E57">
         <v>1</v>
@@ -3031,17 +2820,13 @@
         <v>3.45</v>
       </c>
       <c r="G57" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>3.45</v>
       </c>
-      <c r="H57" s="9">
-        <f t="shared" si="2"/>
-        <v>4.3125</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="E58">
         <v>1</v>
@@ -3050,20 +2835,16 @@
         <v>5</v>
       </c>
       <c r="G58" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="H58" s="9">
-        <f t="shared" si="2"/>
-        <v>6.25</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>210</v>
+        <v>219</v>
       </c>
       <c r="B59" t="s">
-        <v>209</v>
+        <v>218</v>
       </c>
       <c r="E59">
         <v>4</v>
@@ -3072,20 +2853,16 @@
         <v>0.1</v>
       </c>
       <c r="G59" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
-      <c r="H59" s="9">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>211</v>
+        <v>220</v>
       </c>
       <c r="B60" t="s">
-        <v>212</v>
+        <v>221</v>
       </c>
       <c r="E60">
         <v>1</v>
@@ -3094,20 +2871,16 @@
         <v>0.1</v>
       </c>
       <c r="G60" s="9">
-        <f t="shared" ref="G60" si="5">F60*E60</f>
+        <f t="shared" ref="G60" si="3">F60*E60</f>
         <v>0.1</v>
       </c>
-      <c r="H60" s="9">
-        <f t="shared" si="2"/>
-        <v>0.125</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="10" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="B61" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="E61">
         <v>1</v>
@@ -3119,17 +2892,13 @@
         <f>F59*E59</f>
         <v>0.4</v>
       </c>
-      <c r="H61" s="9">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>213</v>
+        <v>222</v>
       </c>
       <c r="B62" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="E62">
         <v>4</v>
@@ -3138,20 +2907,16 @@
         <v>0.1</v>
       </c>
       <c r="G62" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
-      <c r="H62" s="9">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B63" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="E63">
         <v>2</v>
@@ -3160,20 +2925,16 @@
         <v>0.1</v>
       </c>
       <c r="G63" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
-      <c r="H63" s="9">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B64" t="s">
-        <v>233</v>
+        <v>156</v>
       </c>
       <c r="E64">
         <v>1</v>
@@ -3182,46 +2943,38 @@
         <v>1</v>
       </c>
       <c r="G64" s="9">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="H64" s="9">
-        <f t="shared" si="2"/>
-        <v>1.25</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A65" s="7" t="s">
-        <v>246</v>
+        <v>158</v>
       </c>
       <c r="B65" s="7"/>
       <c r="C65" s="7"/>
       <c r="D65" s="7"/>
       <c r="E65" s="7"/>
       <c r="F65" s="7"/>
-      <c r="G65" s="8"/>
-      <c r="H65" s="8">
-        <f>SUM(H62:H64)+SUM(H58:H60)+SUM(H51:H56)+H49</f>
-        <v>43.418750000000003</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A67" s="24" t="s">
-        <v>155</v>
-      </c>
-      <c r="B67" s="24"/>
-      <c r="C67" s="24"/>
-      <c r="D67" s="24"/>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G65" s="8">
+        <f>SUM(G49:G64)</f>
+        <v>43.695000000000007</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A67" s="28" t="s">
+        <v>159</v>
+      </c>
+      <c r="B67" s="28"/>
+      <c r="C67" s="28"/>
+      <c r="D67" s="28"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="B68" t="s">
-        <v>207</v>
-      </c>
-      <c r="C68" s="15" t="s">
-        <v>234</v>
+        <v>216</v>
       </c>
       <c r="E68">
         <v>1</v>
@@ -3229,69 +2982,48 @@
       <c r="F68" s="9">
         <v>171.4</v>
       </c>
-      <c r="G68" s="9">
-        <f t="shared" ref="G68" si="6">F68*E68</f>
+      <c r="G68">
+        <f>F68*E68</f>
         <v>171.4</v>
       </c>
-      <c r="H68">
-        <f>G68*1.25</f>
-        <v>214.25</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F69" s="9"/>
-      <c r="G69" s="9"/>
-    </row>
-    <row r="70" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A70" s="24" t="s">
-        <v>157</v>
-      </c>
-      <c r="B70" s="24"/>
-      <c r="C70" s="24"/>
-      <c r="D70" s="24"/>
-      <c r="G70" s="9"/>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:7" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A70" s="28" t="s">
+        <v>161</v>
+      </c>
+      <c r="B70" s="28"/>
+      <c r="C70" s="28"/>
+      <c r="D70" s="28"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>158</v>
-      </c>
-      <c r="B71" s="15" t="s">
-        <v>235</v>
+        <v>162</v>
       </c>
       <c r="E71">
         <v>1</v>
       </c>
       <c r="F71" s="9">
-        <v>17</v>
-      </c>
-      <c r="G71" s="9">
-        <f>F71*E71</f>
-        <v>17</v>
-      </c>
-      <c r="H71" s="9">
-        <f>G71*1.25</f>
-        <v>21.25</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+        <v>35.06</v>
+      </c>
+      <c r="G71">
+        <v>35.06</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F72" s="9"/>
-      <c r="G72" s="9"/>
-      <c r="H72" s="9"/>
-    </row>
-    <row r="73" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A73" s="24" t="s">
-        <v>159</v>
-      </c>
-      <c r="B73" s="24"/>
-      <c r="G73" s="9"/>
-      <c r="H73" s="9"/>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="73" spans="1:7" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A73" s="28" t="s">
+        <v>163</v>
+      </c>
+      <c r="B73" s="28"/>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>160</v>
-      </c>
-      <c r="B74" t="s">
-        <v>236</v>
+        <v>164</v>
       </c>
       <c r="E74">
         <v>1</v>
@@ -3299,21 +3031,14 @@
       <c r="F74" s="9">
         <v>66.34</v>
       </c>
-      <c r="G74" s="9">
-        <f t="shared" ref="G74:G75" si="7">F74*E74</f>
+      <c r="G74">
+        <f t="shared" ref="G74:G75" si="4">F74*E74</f>
         <v>66.34</v>
       </c>
-      <c r="H74" s="9">
-        <f t="shared" ref="H74:H79" si="8">G74*1.25</f>
-        <v>82.925000000000011</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>237</v>
-      </c>
-      <c r="B75" t="s">
-        <v>238</v>
+        <v>165</v>
       </c>
       <c r="E75">
         <v>1</v>
@@ -3321,83 +3046,64 @@
       <c r="F75" s="9">
         <v>38.340000000000003</v>
       </c>
-      <c r="G75" s="9">
-        <f t="shared" si="7"/>
+      <c r="G75">
+        <f t="shared" si="4"/>
         <v>38.340000000000003</v>
       </c>
-      <c r="H75" s="9">
-        <f t="shared" si="8"/>
-        <v>47.925000000000004</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A76" s="7"/>
-      <c r="F76" s="17"/>
-      <c r="G76" s="17"/>
-      <c r="H76" s="9"/>
-    </row>
-    <row r="77" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A77" s="24" t="s">
-        <v>239</v>
-      </c>
-      <c r="B77" s="24"/>
-      <c r="H77" s="9"/>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>240</v>
-      </c>
-      <c r="B78" t="s">
-        <v>242</v>
-      </c>
-      <c r="E78">
-        <v>1</v>
-      </c>
-      <c r="F78" s="9">
-        <v>18</v>
-      </c>
-      <c r="G78" s="9">
-        <f t="shared" ref="G78:G79" si="9">F78*E78</f>
-        <v>18</v>
-      </c>
-      <c r="H78" s="9">
-        <f t="shared" si="8"/>
-        <v>22.5</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>241</v>
-      </c>
-      <c r="B79" t="s">
-        <v>243</v>
-      </c>
-      <c r="E79">
-        <v>1</v>
-      </c>
-      <c r="F79" s="9">
-        <v>17</v>
-      </c>
-      <c r="G79" s="9">
-        <f t="shared" si="9"/>
-        <v>17</v>
-      </c>
-      <c r="H79" s="9">
-        <f t="shared" si="8"/>
-        <v>21.25</v>
-      </c>
+    </row>
+    <row r="76" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A76" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="F76" s="18">
+        <f>SUM(G74:G75)</f>
+        <v>104.68</v>
+      </c>
+      <c r="G76" s="18"/>
+    </row>
+    <row r="78" spans="1:7" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A78" s="27" t="s">
+        <v>167</v>
+      </c>
+      <c r="B78" s="27"/>
+      <c r="C78" s="27"/>
+      <c r="D78" s="11"/>
+      <c r="E78" s="11"/>
+      <c r="F78" s="19">
+        <f>F76+G65+I46+G68</f>
+        <v>396.66999999999996</v>
+      </c>
+      <c r="G78" s="19"/>
+    </row>
+    <row r="79" spans="1:7" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A79" s="27" t="s">
+        <v>168</v>
+      </c>
+      <c r="B79" s="27"/>
+      <c r="C79" s="27"/>
+      <c r="D79" s="11"/>
+      <c r="E79" s="11"/>
+      <c r="F79" s="19">
+        <f>F76+G65+I46+G71</f>
+        <v>260.33</v>
+      </c>
+      <c r="G79" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="A77:B77"/>
+  <mergeCells count="15">
     <mergeCell ref="F76:G76"/>
+    <mergeCell ref="F78:G78"/>
+    <mergeCell ref="F79:G79"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="A49:C49"/>
+    <mergeCell ref="A79:C79"/>
     <mergeCell ref="A67:B67"/>
     <mergeCell ref="A70:B70"/>
     <mergeCell ref="A73:B73"/>
+    <mergeCell ref="A78:C78"/>
     <mergeCell ref="C67:D67"/>
     <mergeCell ref="C70:D70"/>
   </mergeCells>
@@ -3406,8 +3112,6 @@
     <hyperlink ref="B55" r:id="rId2" xr:uid="{5A33C5A7-DC1C-4D1C-82D4-6F10AD1F10D3}"/>
     <hyperlink ref="B56" r:id="rId3" xr:uid="{537D6D9C-9F20-4B7C-8ECD-54BA77D8ACC7}"/>
     <hyperlink ref="B57" r:id="rId4" xr:uid="{DC7B44C9-7248-43F5-9F3E-3B4750BAB0D5}"/>
-    <hyperlink ref="C68" r:id="rId5" xr:uid="{1D7E88CD-AFAA-4B97-9D92-1ED605380133}"/>
-    <hyperlink ref="B71" r:id="rId6" xr:uid="{51F49AE6-72ED-40A6-BE54-4BFB91B32B23}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>